<commit_message>
playerdata 추가. resaerch 배수데이터 입력전.
</commit_message>
<xml_diff>
--- a/Doc/XmlDataDocument.xlsx
+++ b/Doc/XmlDataDocument.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
   <si>
     <t>R01</t>
   </si>
@@ -190,10 +190,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -338,6 +334,10 @@
   </si>
   <si>
     <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -433,6 +433,36 @@
   <dxfs count="21">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -440,37 +470,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -620,25 +620,25 @@
     <tableColumn id="5" uniqueName="name" name="name" dataDxfId="14">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/Info/@name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="description" name="descrption" dataDxfId="4">
+    <tableColumn id="6" uniqueName="description" name="descrption" dataDxfId="13">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/Info/@description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="value" name="price" dataDxfId="3">
+    <tableColumn id="7" uniqueName="value" name="price" dataDxfId="12">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/Price/@value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="digit" name="pricedigit" dataDxfId="2">
+    <tableColumn id="8" uniqueName="digit" name="pricedigit" dataDxfId="11">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/Price/@digit" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="value" name="potvalue" dataDxfId="0">
+    <tableColumn id="12" uniqueName="value" name="potvalue" dataDxfId="10">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/PriceOverTime/@value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="digit" name="potdigit" dataDxfId="1">
+    <tableColumn id="9" uniqueName="digit" name="potdigit" dataDxfId="9">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/PriceOverTime/@digit" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="time" name="time" dataDxfId="13">
+    <tableColumn id="10" uniqueName="time" name="time" dataDxfId="8">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/PriceOverTime/@time" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="groupid" name="groupid" dataDxfId="12">
+    <tableColumn id="11" uniqueName="groupid" name="groupid" dataDxfId="7">
       <xmlColumnPr mapId="6" xpath="/Researches/Research/BonusList/@groupid" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -647,23 +647,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="표29" displayName="표29" ref="N1:R10" tableType="xml" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" connectionId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="표29" displayName="표29" ref="N1:R10" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="2">
   <autoFilter ref="N1:R10"/>
   <tableColumns count="5">
-    <tableColumn id="1" uniqueName="group" name="group" dataDxfId="9">
+    <tableColumn id="1" uniqueName="group" name="group" dataDxfId="4">
       <calculatedColumnFormula>표28[[#This Row],[groupid]]</calculatedColumnFormula>
       <xmlColumnPr mapId="4" xpath="/BonusList/Bonus/@group" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="target" name="target" dataDxfId="8">
+    <tableColumn id="2" uniqueName="target" name="target" dataDxfId="3">
       <xmlColumnPr mapId="4" xpath="/BonusList/Bonus/@target" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="attribute" name="attribute" dataDxfId="7">
+    <tableColumn id="3" uniqueName="attribute" name="attribute" dataDxfId="2">
       <xmlColumnPr mapId="4" xpath="/BonusList/Bonus/@attribute" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="value" name="value" dataDxfId="6">
+    <tableColumn id="4" uniqueName="value" name="value" dataDxfId="1">
       <xmlColumnPr mapId="4" xpath="/BonusList/Bonus/@value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="stringvalue" name="stringvalue" dataDxfId="5">
+    <tableColumn id="5" uniqueName="stringvalue" name="stringvalue" dataDxfId="0">
       <xmlColumnPr mapId="4" xpath="/BonusList/Bonus/@stringvalue" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -983,7 +983,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1044,19 +1044,19 @@
         <v>8</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1080,13 +1080,13 @@
         <v>22</v>
       </c>
       <c r="G2" s="7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>42</v>
+      <c r="I2" s="7">
+        <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>39</v>
@@ -1103,16 +1103,16 @@
         <v>BR01</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q2" s="2">
         <v>1</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1136,13 +1136,13 @@
         <v>23</v>
       </c>
       <c r="G3" s="7">
-        <v>25</v>
+        <v>500</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="7">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>39</v>
@@ -1159,16 +1159,16 @@
         <v>BR02</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q3" s="2">
         <v>1</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1192,13 +1192,13 @@
         <v>32</v>
       </c>
       <c r="G4" s="7">
-        <v>500</v>
+        <v>33333</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="7">
-        <v>25</v>
+        <v>1250</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>39</v>
@@ -1215,16 +1215,16 @@
         <v>BR03</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q4" s="2">
         <v>1</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1248,16 +1248,16 @@
         <v>33</v>
       </c>
       <c r="G5" s="7">
-        <v>33333</v>
+        <v>2300</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="I5" s="7">
-        <v>1250</v>
+        <v>90</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="K5" s="2">
         <v>60</v>
@@ -1271,16 +1271,16 @@
         <v>BR04</v>
       </c>
       <c r="O5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q5" s="2">
         <v>1</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1304,16 +1304,16 @@
         <v>34</v>
       </c>
       <c r="G6" s="7">
-        <v>2300</v>
+        <v>1850</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="I6" s="7">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K6" s="2">
         <v>60</v>
@@ -1327,16 +1327,16 @@
         <v>BR05</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q6" s="2">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -1360,16 +1360,16 @@
         <v>35</v>
       </c>
       <c r="G7" s="7">
-        <v>1850</v>
+        <v>1100</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>73</v>
       </c>
       <c r="I7" s="7">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K7" s="2">
         <v>60</v>
@@ -1383,16 +1383,16 @@
         <v>BR06</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q7" s="2">
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -1416,16 +1416,16 @@
         <v>36</v>
       </c>
       <c r="G8" s="7">
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I8" s="7">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K8" s="2">
         <v>60</v>
@@ -1439,16 +1439,16 @@
         <v>BR07</v>
       </c>
       <c r="O8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q8" s="2">
         <v>1</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1472,13 +1472,13 @@
         <v>37</v>
       </c>
       <c r="G9" s="7">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>78</v>
       </c>
       <c r="I9" s="7">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>80</v>
@@ -1495,16 +1495,16 @@
         <v>BR08</v>
       </c>
       <c r="O9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q9" s="2">
         <v>1</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1528,13 +1528,13 @@
         <v>38</v>
       </c>
       <c r="G10" s="7">
-        <v>850</v>
+        <v>1800</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I10" s="7">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>81</v>
@@ -1551,16 +1551,16 @@
         <v>BR09</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="Q10" s="2">
         <v>1</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1638,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:H10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1654,172 +1654,172 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>5200</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3.3361999999999998</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>5300</v>
       </c>
       <c r="D3">
-        <v>3.3361999999999998</v>
+        <v>36.895000000000003</v>
       </c>
       <c r="E3">
-        <v>86</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4">
         <v>5500</v>
       </c>
-      <c r="D4">
-        <v>36.895000000000003</v>
+      <c r="D4" s="5">
+        <v>1017.7</v>
       </c>
       <c r="E4">
-        <v>2001</v>
+        <v>108544.00000000048</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>5700</v>
       </c>
-      <c r="D5" s="5">
-        <v>1017.7</v>
+      <c r="D5">
+        <v>39766</v>
       </c>
       <c r="E5">
-        <v>108544.00000000048</v>
+        <v>7733248</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>6100</v>
       </c>
       <c r="D6">
-        <v>39766</v>
+        <v>15589731</v>
       </c>
       <c r="E6">
-        <v>7733248</v>
+        <v>6056866302</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>6300</v>
       </c>
       <c r="D7">
-        <v>15589731</v>
+        <v>4990733267</v>
       </c>
       <c r="E7">
-        <v>6056866302</v>
+        <v>3509157065962</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>6700</v>
       </c>
       <c r="D8">
-        <v>4990733267</v>
+        <v>1677322427419</v>
       </c>
       <c r="E8">
-        <v>3509157065962</v>
+        <v>2005605675653396</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>6900</v>
       </c>
       <c r="D9">
-        <v>1677322427419</v>
+        <v>1312779264637361.5</v>
       </c>
       <c r="E9">
-        <v>2005605675653396</v>
+        <v>2.6376361699820129E+18</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>7300</v>
       </c>
-      <c r="D10">
-        <v>1312779264637361.5</v>
+      <c r="D10" s="5">
+        <v>1.9356116650602877E+18</v>
       </c>
       <c r="E10">
-        <v>2.6376361699820129E+18</v>
+        <v>6.0169996591185768E+21</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1828,6 +1828,9 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "리서치 시스템 완료 ㅠㅠ"""
This reverts commit 78bc8c5c76d9ec54384014666e3130e01521bfd4.
</commit_message>
<xml_diff>
--- a/Doc/XmlDataDocument.xlsx
+++ b/Doc/XmlDataDocument.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="516">
   <si>
     <t>R01</t>
   </si>
@@ -1651,141 +1651,6 @@
   <si>
     <t>DpcX</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R00_046</t>
-  </si>
-  <si>
-    <t>R00_047</t>
-  </si>
-  <si>
-    <t>R00_048</t>
-  </si>
-  <si>
-    <t>R00_049</t>
-  </si>
-  <si>
-    <t>R00_050</t>
-  </si>
-  <si>
-    <t>R00_051</t>
-  </si>
-  <si>
-    <t>R00_052</t>
-  </si>
-  <si>
-    <t>R00_053</t>
-  </si>
-  <si>
-    <t>R00_054</t>
-  </si>
-  <si>
-    <t>R00_055</t>
-  </si>
-  <si>
-    <t>R00_056</t>
-  </si>
-  <si>
-    <t>R00_057</t>
-  </si>
-  <si>
-    <t>R00_058</t>
-  </si>
-  <si>
-    <t>R00_059</t>
-  </si>
-  <si>
-    <t>R00_060</t>
-  </si>
-  <si>
-    <t>R00_061</t>
-  </si>
-  <si>
-    <t>R00_062</t>
-  </si>
-  <si>
-    <t>R00_063</t>
-  </si>
-  <si>
-    <t>R00_064</t>
-  </si>
-  <si>
-    <t>R00_065</t>
-  </si>
-  <si>
-    <t>R00_066</t>
-  </si>
-  <si>
-    <t>R00_067</t>
-  </si>
-  <si>
-    <t>R00_068</t>
-  </si>
-  <si>
-    <t>R00_069</t>
-  </si>
-  <si>
-    <t>R00_070</t>
-  </si>
-  <si>
-    <t>R00_071</t>
-  </si>
-  <si>
-    <t>R00_072</t>
-  </si>
-  <si>
-    <t>R00_073</t>
-  </si>
-  <si>
-    <t>R00_074</t>
-  </si>
-  <si>
-    <t>R00_075</t>
-  </si>
-  <si>
-    <t>R00_076</t>
-  </si>
-  <si>
-    <t>R00_077</t>
-  </si>
-  <si>
-    <t>R00_078</t>
-  </si>
-  <si>
-    <t>R00_079</t>
-  </si>
-  <si>
-    <t>R00_080</t>
-  </si>
-  <si>
-    <t>R00_081</t>
-  </si>
-  <si>
-    <t>R00_082</t>
-  </si>
-  <si>
-    <t>R00_083</t>
-  </si>
-  <si>
-    <t>R00_084</t>
-  </si>
-  <si>
-    <t>R00_085</t>
-  </si>
-  <si>
-    <t>R00_086</t>
-  </si>
-  <si>
-    <t>R00_087</t>
-  </si>
-  <si>
-    <t>R00_088</t>
-  </si>
-  <si>
-    <t>R00_089</t>
-  </si>
-  <si>
-    <t>R00_090</t>
   </si>
 </sst>
 </file>
@@ -1817,18 +1682,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1845,7 +1704,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1871,33 +1730,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2073,8 +1905,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="표28" displayName="표28" ref="A1:L505" tableType="xml" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" connectionId="8">
-  <autoFilter ref="A1:L505">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="표28" displayName="표28" ref="A1:L460" tableType="xml" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" connectionId="8">
+  <autoFilter ref="A1:L460">
     <filterColumn colId="8"/>
     <filterColumn colId="10"/>
     <filterColumn colId="11"/>
@@ -2123,8 +1955,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="표29" displayName="표29" ref="N1:R505" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="2">
-  <autoFilter ref="N1:R505"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="표29" displayName="표29" ref="N1:R460" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="2">
+  <autoFilter ref="N1:R460"/>
   <tableColumns count="5">
     <tableColumn id="1" uniqueName="group" name="group" dataDxfId="4">
       <calculatedColumnFormula>표28[[#This Row],[groupid]]</calculatedColumnFormula>
@@ -2456,13 +2288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R505"/>
+  <dimension ref="A1:R460"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A411" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J428" sqref="J428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2572,7 +2401,7 @@
         <v>70</v>
       </c>
       <c r="K2" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2626,7 +2455,7 @@
         <v>70</v>
       </c>
       <c r="K3" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2680,7 +2509,7 @@
         <v>70</v>
       </c>
       <c r="K4" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2734,7 +2563,7 @@
         <v>70</v>
       </c>
       <c r="K5" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L5" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2788,7 +2617,7 @@
         <v>70</v>
       </c>
       <c r="K6" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L6" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2842,7 +2671,7 @@
         <v>70</v>
       </c>
       <c r="K7" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L7" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2896,7 +2725,7 @@
         <v>70</v>
       </c>
       <c r="K8" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2950,7 +2779,7 @@
         <v>70</v>
       </c>
       <c r="K9" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -3004,7 +2833,7 @@
         <v>70</v>
       </c>
       <c r="K10" s="2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="L10" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -3130,7 +2959,7 @@
         <v>101</v>
       </c>
       <c r="Q12" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -3184,7 +3013,7 @@
         <v>101</v>
       </c>
       <c r="Q13" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -3238,7 +3067,7 @@
         <v>101</v>
       </c>
       <c r="Q14" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -3292,7 +3121,7 @@
         <v>101</v>
       </c>
       <c r="Q15" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -3616,7 +3445,7 @@
         <v>101</v>
       </c>
       <c r="Q21" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -3670,7 +3499,7 @@
         <v>101</v>
       </c>
       <c r="Q22" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -3724,7 +3553,7 @@
         <v>101</v>
       </c>
       <c r="Q23" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -3778,7 +3607,7 @@
         <v>101</v>
       </c>
       <c r="Q24" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -3832,7 +3661,7 @@
         <v>101</v>
       </c>
       <c r="Q25" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -3886,7 +3715,7 @@
         <v>101</v>
       </c>
       <c r="Q26" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -3940,7 +3769,7 @@
         <v>101</v>
       </c>
       <c r="Q27" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -3994,7 +3823,7 @@
         <v>101</v>
       </c>
       <c r="Q28" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -4048,7 +3877,7 @@
         <v>101</v>
       </c>
       <c r="Q29" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -4102,7 +3931,7 @@
         <v>101</v>
       </c>
       <c r="Q30" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -4156,7 +3985,7 @@
         <v>101</v>
       </c>
       <c r="Q31" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -4372,7 +4201,7 @@
         <v>101</v>
       </c>
       <c r="Q35" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -4534,7 +4363,7 @@
         <v>101</v>
       </c>
       <c r="Q38" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -4588,7 +4417,7 @@
         <v>101</v>
       </c>
       <c r="Q39" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -4642,7 +4471,7 @@
         <v>101</v>
       </c>
       <c r="Q40" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -4696,7 +4525,7 @@
         <v>101</v>
       </c>
       <c r="Q41" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -7102,7 +6931,7 @@
         <v>101</v>
       </c>
       <c r="Q85" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="R85" s="7"/>
     </row>
@@ -9412,7 +9241,7 @@
         <v>101</v>
       </c>
       <c r="Q127" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="R127" s="7"/>
     </row>
@@ -9467,7 +9296,7 @@
         <v>101</v>
       </c>
       <c r="Q128" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="R128" s="7"/>
     </row>
@@ -25264,7 +25093,7 @@
         <v>505</v>
       </c>
       <c r="C416" s="7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D416" s="1" t="s">
         <v>514</v>
@@ -25278,7 +25107,7 @@
         <v>@SR00_001D@</v>
       </c>
       <c r="G416" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H416" s="8">
         <v>0</v>
@@ -25319,7 +25148,7 @@
         <v>505</v>
       </c>
       <c r="C417" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D417" s="1" t="s">
         <v>514</v>
@@ -25333,7 +25162,7 @@
         <v>@SR00_002D@</v>
       </c>
       <c r="G417" s="5">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H417" s="8">
         <v>0</v>
@@ -25362,7 +25191,7 @@
         <v>515</v>
       </c>
       <c r="Q417" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R417" s="7"/>
     </row>
@@ -25374,7 +25203,7 @@
         <v>505</v>
       </c>
       <c r="C418" s="7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D418" s="1" t="s">
         <v>513</v>
@@ -25388,7 +25217,7 @@
         <v>@SR00_003D@</v>
       </c>
       <c r="G418" s="8">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H418" s="8">
         <v>0</v>
@@ -25417,7 +25246,7 @@
         <v>515</v>
       </c>
       <c r="Q418" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R418" s="7"/>
     </row>
@@ -25429,7 +25258,7 @@
         <v>505</v>
       </c>
       <c r="C419" s="2">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D419" s="1" t="s">
         <v>513</v>
@@ -25443,7 +25272,7 @@
         <v>@SR00_004D@</v>
       </c>
       <c r="G419" s="5">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="H419" s="8">
         <v>0</v>
@@ -25472,7 +25301,7 @@
         <v>515</v>
       </c>
       <c r="Q419" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="R419" s="7"/>
     </row>
@@ -25484,7 +25313,7 @@
         <v>505</v>
       </c>
       <c r="C420" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D420" s="1" t="s">
         <v>513</v>
@@ -25498,7 +25327,7 @@
         <v>@SR00_005D@</v>
       </c>
       <c r="G420" s="8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H420" s="8">
         <v>0</v>
@@ -25527,7 +25356,7 @@
         <v>515</v>
       </c>
       <c r="Q420" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R420" s="7"/>
     </row>
@@ -25539,7 +25368,7 @@
         <v>505</v>
       </c>
       <c r="C421" s="2">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D421" s="1" t="s">
         <v>513</v>
@@ -25553,7 +25382,7 @@
         <v>@SR00_006D@</v>
       </c>
       <c r="G421" s="5">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="H421" s="8">
         <v>0</v>
@@ -25582,7 +25411,7 @@
         <v>515</v>
       </c>
       <c r="Q421" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R421" s="7"/>
     </row>
@@ -25594,7 +25423,7 @@
         <v>505</v>
       </c>
       <c r="C422" s="7">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="D422" s="1" t="s">
         <v>513</v>
@@ -25608,7 +25437,7 @@
         <v>@SR00_007D@</v>
       </c>
       <c r="G422" s="8">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="H422" s="8">
         <v>0</v>
@@ -25637,7 +25466,7 @@
         <v>515</v>
       </c>
       <c r="Q422" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R422" s="7"/>
     </row>
@@ -25649,7 +25478,7 @@
         <v>505</v>
       </c>
       <c r="C423" s="2">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="D423" s="1" t="s">
         <v>513</v>
@@ -25663,7 +25492,7 @@
         <v>@SR00_008D@</v>
       </c>
       <c r="G423" s="5">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="H423" s="8">
         <v>0</v>
@@ -25692,7 +25521,7 @@
         <v>515</v>
       </c>
       <c r="Q423" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R423" s="7"/>
     </row>
@@ -25704,7 +25533,7 @@
         <v>505</v>
       </c>
       <c r="C424" s="7">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="D424" s="1" t="s">
         <v>513</v>
@@ -25718,7 +25547,7 @@
         <v>@SR00_009D@</v>
       </c>
       <c r="G424" s="8">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H424" s="8">
         <v>0</v>
@@ -25747,7 +25576,7 @@
         <v>515</v>
       </c>
       <c r="Q424" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R424" s="7"/>
     </row>
@@ -25759,7 +25588,7 @@
         <v>505</v>
       </c>
       <c r="C425" s="2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D425" s="1" t="s">
         <v>513</v>
@@ -25773,7 +25602,7 @@
         <v>@SR00_010D@</v>
       </c>
       <c r="G425" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H425" s="8">
         <v>0</v>
@@ -25802,7 +25631,7 @@
         <v>515</v>
       </c>
       <c r="Q425" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R425" s="7"/>
     </row>
@@ -25814,7 +25643,7 @@
         <v>505</v>
       </c>
       <c r="C426" s="7">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="D426" s="1" t="s">
         <v>513</v>
@@ -25828,7 +25657,7 @@
         <v>@SR00_011D@</v>
       </c>
       <c r="G426" s="8">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="H426" s="8">
         <v>0</v>
@@ -25857,7 +25686,7 @@
         <v>515</v>
       </c>
       <c r="Q426" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R426" s="7"/>
     </row>
@@ -25869,7 +25698,7 @@
         <v>505</v>
       </c>
       <c r="C427" s="2">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D427" s="1" t="s">
         <v>513</v>
@@ -25883,7 +25712,7 @@
         <v>@SR00_012D@</v>
       </c>
       <c r="G427" s="5">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="H427" s="8">
         <v>0</v>
@@ -25912,7 +25741,7 @@
         <v>515</v>
       </c>
       <c r="Q427" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R427" s="7"/>
     </row>
@@ -25924,7 +25753,7 @@
         <v>505</v>
       </c>
       <c r="C428" s="7">
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="D428" s="1" t="s">
         <v>513</v>
@@ -25938,7 +25767,7 @@
         <v>@SR00_013D@</v>
       </c>
       <c r="G428" s="8">
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="H428" s="8">
         <v>0</v>
@@ -25967,7 +25796,7 @@
         <v>515</v>
       </c>
       <c r="Q428" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R428" s="7"/>
     </row>
@@ -25979,7 +25808,7 @@
         <v>505</v>
       </c>
       <c r="C429" s="2">
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="D429" s="1" t="s">
         <v>513</v>
@@ -25993,7 +25822,7 @@
         <v>@SR00_014D@</v>
       </c>
       <c r="G429" s="5">
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="H429" s="8">
         <v>0</v>
@@ -26022,7 +25851,7 @@
         <v>515</v>
       </c>
       <c r="Q429" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="R429" s="7"/>
     </row>
@@ -26034,7 +25863,7 @@
         <v>505</v>
       </c>
       <c r="C430" s="7">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D430" s="1" t="s">
         <v>513</v>
@@ -26048,7 +25877,7 @@
         <v>@SR00_015D@</v>
       </c>
       <c r="G430" s="8">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H430" s="8">
         <v>0</v>
@@ -26077,7 +25906,7 @@
         <v>515</v>
       </c>
       <c r="Q430" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="R430" s="7"/>
     </row>
@@ -26089,7 +25918,7 @@
         <v>505</v>
       </c>
       <c r="C431" s="2">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D431" s="1" t="s">
         <v>513</v>
@@ -26103,7 +25932,7 @@
         <v>@SR00_016D@</v>
       </c>
       <c r="G431" s="5">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="H431" s="8">
         <v>0</v>
@@ -26132,7 +25961,7 @@
         <v>515</v>
       </c>
       <c r="Q431" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="R431" s="7"/>
     </row>
@@ -26144,7 +25973,7 @@
         <v>505</v>
       </c>
       <c r="C432" s="7">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="D432" s="1" t="s">
         <v>513</v>
@@ -26158,7 +25987,7 @@
         <v>@SR00_017D@</v>
       </c>
       <c r="G432" s="8">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="H432" s="8">
         <v>0</v>
@@ -26187,7 +26016,7 @@
         <v>515</v>
       </c>
       <c r="Q432" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="R432" s="7"/>
     </row>
@@ -26199,7 +26028,7 @@
         <v>505</v>
       </c>
       <c r="C433" s="2">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="D433" s="1" t="s">
         <v>513</v>
@@ -26213,7 +26042,7 @@
         <v>@SR00_018D@</v>
       </c>
       <c r="G433" s="5">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="H433" s="8">
         <v>0</v>
@@ -26242,7 +26071,7 @@
         <v>515</v>
       </c>
       <c r="Q433" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="R433" s="7"/>
     </row>
@@ -26254,7 +26083,7 @@
         <v>505</v>
       </c>
       <c r="C434" s="7">
-        <v>190</v>
+        <v>380</v>
       </c>
       <c r="D434" s="1" t="s">
         <v>513</v>
@@ -26268,7 +26097,7 @@
         <v>@SR00_019D@</v>
       </c>
       <c r="G434" s="8">
-        <v>190</v>
+        <v>380</v>
       </c>
       <c r="H434" s="8">
         <v>0</v>
@@ -26297,7 +26126,7 @@
         <v>515</v>
       </c>
       <c r="Q434" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="R434" s="7"/>
     </row>
@@ -26309,7 +26138,7 @@
         <v>505</v>
       </c>
       <c r="C435" s="2">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="D435" s="1" t="s">
         <v>513</v>
@@ -26323,7 +26152,7 @@
         <v>@SR00_020D@</v>
       </c>
       <c r="G435" s="5">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="H435" s="8">
         <v>0</v>
@@ -26352,7 +26181,7 @@
         <v>515</v>
       </c>
       <c r="Q435" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="R435" s="7"/>
     </row>
@@ -26364,7 +26193,7 @@
         <v>505</v>
       </c>
       <c r="C436" s="7">
-        <v>210</v>
+        <v>420</v>
       </c>
       <c r="D436" s="1" t="s">
         <v>513</v>
@@ -26378,7 +26207,7 @@
         <v>@SR00_021D@</v>
       </c>
       <c r="G436" s="8">
-        <v>210</v>
+        <v>420</v>
       </c>
       <c r="H436" s="8">
         <v>0</v>
@@ -26407,7 +26236,7 @@
         <v>515</v>
       </c>
       <c r="Q436" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="R436" s="7"/>
     </row>
@@ -26419,7 +26248,7 @@
         <v>505</v>
       </c>
       <c r="C437" s="2">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="D437" s="1" t="s">
         <v>513</v>
@@ -26433,7 +26262,7 @@
         <v>@SR00_022D@</v>
       </c>
       <c r="G437" s="5">
-        <v>220</v>
+        <v>440</v>
       </c>
       <c r="H437" s="8">
         <v>0</v>
@@ -26462,7 +26291,7 @@
         <v>515</v>
       </c>
       <c r="Q437" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="R437" s="7"/>
     </row>
@@ -26474,7 +26303,7 @@
         <v>505</v>
       </c>
       <c r="C438" s="7">
-        <v>230</v>
+        <v>460</v>
       </c>
       <c r="D438" s="1" t="s">
         <v>513</v>
@@ -26488,7 +26317,7 @@
         <v>@SR00_023D@</v>
       </c>
       <c r="G438" s="8">
-        <v>230</v>
+        <v>460</v>
       </c>
       <c r="H438" s="8">
         <v>0</v>
@@ -26517,7 +26346,7 @@
         <v>515</v>
       </c>
       <c r="Q438" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="R438" s="7"/>
     </row>
@@ -26529,7 +26358,7 @@
         <v>505</v>
       </c>
       <c r="C439" s="2">
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="D439" s="1" t="s">
         <v>513</v>
@@ -26543,7 +26372,7 @@
         <v>@SR00_024D@</v>
       </c>
       <c r="G439" s="5">
-        <v>240</v>
+        <v>480</v>
       </c>
       <c r="H439" s="8">
         <v>0</v>
@@ -26572,7 +26401,7 @@
         <v>515</v>
       </c>
       <c r="Q439" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="R439" s="7"/>
     </row>
@@ -26584,7 +26413,7 @@
         <v>505</v>
       </c>
       <c r="C440" s="7">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="D440" s="1" t="s">
         <v>513</v>
@@ -26598,7 +26427,7 @@
         <v>@SR00_025D@</v>
       </c>
       <c r="G440" s="8">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="H440" s="8">
         <v>0</v>
@@ -26627,7 +26456,7 @@
         <v>515</v>
       </c>
       <c r="Q440" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="R440" s="7"/>
     </row>
@@ -26639,7 +26468,7 @@
         <v>505</v>
       </c>
       <c r="C441" s="2">
-        <v>260</v>
+        <v>520</v>
       </c>
       <c r="D441" s="1" t="s">
         <v>513</v>
@@ -26653,7 +26482,7 @@
         <v>@SR00_026D@</v>
       </c>
       <c r="G441" s="5">
-        <v>260</v>
+        <v>520</v>
       </c>
       <c r="H441" s="8">
         <v>0</v>
@@ -26682,7 +26511,7 @@
         <v>515</v>
       </c>
       <c r="Q441" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="R441" s="7"/>
     </row>
@@ -26694,7 +26523,7 @@
         <v>505</v>
       </c>
       <c r="C442" s="7">
-        <v>270</v>
+        <v>540</v>
       </c>
       <c r="D442" s="1" t="s">
         <v>513</v>
@@ -26708,7 +26537,7 @@
         <v>@SR00_027D@</v>
       </c>
       <c r="G442" s="8">
-        <v>270</v>
+        <v>540</v>
       </c>
       <c r="H442" s="8">
         <v>0</v>
@@ -26737,7 +26566,7 @@
         <v>515</v>
       </c>
       <c r="Q442" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R442" s="7"/>
     </row>
@@ -26749,7 +26578,7 @@
         <v>505</v>
       </c>
       <c r="C443" s="2">
-        <v>280</v>
+        <v>560</v>
       </c>
       <c r="D443" s="1" t="s">
         <v>513</v>
@@ -26763,7 +26592,7 @@
         <v>@SR00_028D@</v>
       </c>
       <c r="G443" s="5">
-        <v>280</v>
+        <v>560</v>
       </c>
       <c r="H443" s="8">
         <v>0</v>
@@ -26792,7 +26621,7 @@
         <v>515</v>
       </c>
       <c r="Q443" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R443" s="7"/>
     </row>
@@ -26804,7 +26633,7 @@
         <v>505</v>
       </c>
       <c r="C444" s="7">
-        <v>290</v>
+        <v>580</v>
       </c>
       <c r="D444" s="1" t="s">
         <v>513</v>
@@ -26818,7 +26647,7 @@
         <v>@SR00_029D@</v>
       </c>
       <c r="G444" s="8">
-        <v>290</v>
+        <v>580</v>
       </c>
       <c r="H444" s="8">
         <v>0</v>
@@ -26847,7 +26676,7 @@
         <v>515</v>
       </c>
       <c r="Q444" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R444" s="7"/>
     </row>
@@ -26859,7 +26688,7 @@
         <v>505</v>
       </c>
       <c r="C445" s="2">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="D445" s="1" t="s">
         <v>513</v>
@@ -26873,7 +26702,7 @@
         <v>@SR00_030D@</v>
       </c>
       <c r="G445" s="5">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="H445" s="8">
         <v>0</v>
@@ -26902,7 +26731,7 @@
         <v>515</v>
       </c>
       <c r="Q445" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R445" s="7"/>
     </row>
@@ -26914,7 +26743,7 @@
         <v>505</v>
       </c>
       <c r="C446" s="7">
-        <v>310</v>
+        <v>620</v>
       </c>
       <c r="D446" s="1" t="s">
         <v>513</v>
@@ -26928,7 +26757,7 @@
         <v>@SR00_031D@</v>
       </c>
       <c r="G446" s="8">
-        <v>310</v>
+        <v>620</v>
       </c>
       <c r="H446" s="8">
         <v>0</v>
@@ -26957,7 +26786,7 @@
         <v>515</v>
       </c>
       <c r="Q446" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R446" s="7"/>
     </row>
@@ -26969,7 +26798,7 @@
         <v>505</v>
       </c>
       <c r="C447" s="2">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="D447" s="1" t="s">
         <v>513</v>
@@ -26983,7 +26812,7 @@
         <v>@SR00_032D@</v>
       </c>
       <c r="G447" s="5">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="H447" s="8">
         <v>0</v>
@@ -27012,7 +26841,7 @@
         <v>515</v>
       </c>
       <c r="Q447" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R447" s="7"/>
     </row>
@@ -27024,7 +26853,7 @@
         <v>505</v>
       </c>
       <c r="C448" s="7">
-        <v>330</v>
+        <v>660</v>
       </c>
       <c r="D448" s="1" t="s">
         <v>513</v>
@@ -27038,7 +26867,7 @@
         <v>@SR00_033D@</v>
       </c>
       <c r="G448" s="8">
-        <v>330</v>
+        <v>660</v>
       </c>
       <c r="H448" s="8">
         <v>0</v>
@@ -27067,7 +26896,7 @@
         <v>515</v>
       </c>
       <c r="Q448" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R448" s="7"/>
     </row>
@@ -27079,7 +26908,7 @@
         <v>505</v>
       </c>
       <c r="C449" s="2">
-        <v>340</v>
+        <v>680</v>
       </c>
       <c r="D449" s="1" t="s">
         <v>513</v>
@@ -27093,7 +26922,7 @@
         <v>@SR00_034D@</v>
       </c>
       <c r="G449" s="5">
-        <v>340</v>
+        <v>680</v>
       </c>
       <c r="H449" s="8">
         <v>0</v>
@@ -27122,7 +26951,7 @@
         <v>515</v>
       </c>
       <c r="Q449" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R449" s="7"/>
     </row>
@@ -27134,7 +26963,7 @@
         <v>505</v>
       </c>
       <c r="C450" s="7">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="D450" s="1" t="s">
         <v>513</v>
@@ -27148,7 +26977,7 @@
         <v>@SR00_035D@</v>
       </c>
       <c r="G450" s="8">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="H450" s="8">
         <v>0</v>
@@ -27177,7 +27006,7 @@
         <v>515</v>
       </c>
       <c r="Q450" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R450" s="7"/>
     </row>
@@ -27189,7 +27018,7 @@
         <v>505</v>
       </c>
       <c r="C451" s="2">
-        <v>360</v>
+        <v>720</v>
       </c>
       <c r="D451" s="1" t="s">
         <v>513</v>
@@ -27203,7 +27032,7 @@
         <v>@SR00_036D@</v>
       </c>
       <c r="G451" s="5">
-        <v>360</v>
+        <v>720</v>
       </c>
       <c r="H451" s="8">
         <v>0</v>
@@ -27232,7 +27061,7 @@
         <v>515</v>
       </c>
       <c r="Q451" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R451" s="7"/>
     </row>
@@ -27244,7 +27073,7 @@
         <v>505</v>
       </c>
       <c r="C452" s="7">
-        <v>370</v>
+        <v>740</v>
       </c>
       <c r="D452" s="1" t="s">
         <v>513</v>
@@ -27258,7 +27087,7 @@
         <v>@SR00_037D@</v>
       </c>
       <c r="G452" s="8">
-        <v>370</v>
+        <v>740</v>
       </c>
       <c r="H452" s="8">
         <v>0</v>
@@ -27287,7 +27116,7 @@
         <v>515</v>
       </c>
       <c r="Q452" s="2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="R452" s="7"/>
     </row>
@@ -27299,7 +27128,7 @@
         <v>505</v>
       </c>
       <c r="C453" s="2">
-        <v>380</v>
+        <v>760</v>
       </c>
       <c r="D453" s="1" t="s">
         <v>513</v>
@@ -27313,7 +27142,7 @@
         <v>@SR00_038D@</v>
       </c>
       <c r="G453" s="5">
-        <v>380</v>
+        <v>760</v>
       </c>
       <c r="H453" s="8">
         <v>0</v>
@@ -27342,7 +27171,7 @@
         <v>515</v>
       </c>
       <c r="Q453" s="2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="R453" s="7"/>
     </row>
@@ -27354,7 +27183,7 @@
         <v>505</v>
       </c>
       <c r="C454" s="7">
-        <v>390</v>
+        <v>780</v>
       </c>
       <c r="D454" s="1" t="s">
         <v>513</v>
@@ -27368,7 +27197,7 @@
         <v>@SR00_039D@</v>
       </c>
       <c r="G454" s="8">
-        <v>390</v>
+        <v>780</v>
       </c>
       <c r="H454" s="8">
         <v>0</v>
@@ -27397,7 +27226,7 @@
         <v>515</v>
       </c>
       <c r="Q454" s="2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="R454" s="7"/>
     </row>
@@ -27409,7 +27238,7 @@
         <v>505</v>
       </c>
       <c r="C455" s="2">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="D455" s="1" t="s">
         <v>513</v>
@@ -27423,7 +27252,7 @@
         <v>@SR00_040D@</v>
       </c>
       <c r="G455" s="5">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="H455" s="8">
         <v>0</v>
@@ -27452,7 +27281,7 @@
         <v>515</v>
       </c>
       <c r="Q455" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R455" s="7"/>
     </row>
@@ -27464,7 +27293,7 @@
         <v>505</v>
       </c>
       <c r="C456" s="7">
-        <v>410</v>
+        <v>820</v>
       </c>
       <c r="D456" s="1" t="s">
         <v>513</v>
@@ -27478,7 +27307,7 @@
         <v>@SR00_041D@</v>
       </c>
       <c r="G456" s="8">
-        <v>410</v>
+        <v>820</v>
       </c>
       <c r="H456" s="8">
         <v>0</v>
@@ -27507,7 +27336,7 @@
         <v>515</v>
       </c>
       <c r="Q456" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R456" s="7"/>
     </row>
@@ -27519,7 +27348,7 @@
         <v>505</v>
       </c>
       <c r="C457" s="2">
-        <v>420</v>
+        <v>840</v>
       </c>
       <c r="D457" s="1" t="s">
         <v>513</v>
@@ -27533,7 +27362,7 @@
         <v>@SR00_042D@</v>
       </c>
       <c r="G457" s="5">
-        <v>420</v>
+        <v>840</v>
       </c>
       <c r="H457" s="8">
         <v>0</v>
@@ -27562,7 +27391,7 @@
         <v>515</v>
       </c>
       <c r="Q457" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R457" s="7"/>
     </row>
@@ -27574,7 +27403,7 @@
         <v>505</v>
       </c>
       <c r="C458" s="7">
-        <v>430</v>
+        <v>860</v>
       </c>
       <c r="D458" s="1" t="s">
         <v>513</v>
@@ -27588,7 +27417,7 @@
         <v>@SR00_043D@</v>
       </c>
       <c r="G458" s="8">
-        <v>430</v>
+        <v>860</v>
       </c>
       <c r="H458" s="8">
         <v>0</v>
@@ -27617,7 +27446,7 @@
         <v>515</v>
       </c>
       <c r="Q458" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R458" s="7"/>
     </row>
@@ -27629,7 +27458,7 @@
         <v>505</v>
       </c>
       <c r="C459" s="2">
-        <v>440</v>
+        <v>880</v>
       </c>
       <c r="D459" s="1" t="s">
         <v>513</v>
@@ -27643,7 +27472,7 @@
         <v>@SR00_044D@</v>
       </c>
       <c r="G459" s="5">
-        <v>440</v>
+        <v>880</v>
       </c>
       <c r="H459" s="8">
         <v>0</v>
@@ -27672,7 +27501,7 @@
         <v>515</v>
       </c>
       <c r="Q459" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R459" s="7"/>
     </row>
@@ -27684,7 +27513,7 @@
         <v>505</v>
       </c>
       <c r="C460" s="7">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="D460" s="1" t="s">
         <v>513</v>
@@ -27698,7 +27527,7 @@
         <v>@SR00_045D@</v>
       </c>
       <c r="G460" s="8">
-        <v>450</v>
+        <v>900</v>
       </c>
       <c r="H460" s="8">
         <v>0</v>
@@ -27727,2484 +27556,9 @@
         <v>515</v>
       </c>
       <c r="Q460" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R460" s="7"/>
-    </row>
-    <row r="461" spans="1:18">
-      <c r="A461" s="7" t="s">
-        <v>516</v>
-      </c>
-      <c r="B461" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C461" s="2">
-        <v>460</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="E461" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_046N@</v>
-      </c>
-      <c r="F461" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_046D@</v>
-      </c>
-      <c r="G461" s="5">
-        <v>460</v>
-      </c>
-      <c r="H461" s="8">
-        <v>0</v>
-      </c>
-      <c r="I461" s="8">
-        <v>50</v>
-      </c>
-      <c r="J461" s="7">
-        <v>70</v>
-      </c>
-      <c r="K461" s="7">
-        <v>30</v>
-      </c>
-      <c r="L461" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_046</v>
-      </c>
-      <c r="N461" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_046</v>
-      </c>
-      <c r="O461" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P461" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q461" s="2">
-        <v>4</v>
-      </c>
-      <c r="R461" s="7"/>
-    </row>
-    <row r="462" spans="1:18">
-      <c r="A462" s="7" t="s">
-        <v>517</v>
-      </c>
-      <c r="B462" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C462" s="7">
-        <v>470</v>
-      </c>
-      <c r="D462" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="E462" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_047N@</v>
-      </c>
-      <c r="F462" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_047D@</v>
-      </c>
-      <c r="G462" s="8">
-        <v>470</v>
-      </c>
-      <c r="H462" s="8">
-        <v>0</v>
-      </c>
-      <c r="I462" s="8">
-        <v>50</v>
-      </c>
-      <c r="J462" s="7">
-        <v>70</v>
-      </c>
-      <c r="K462" s="7">
-        <v>30</v>
-      </c>
-      <c r="L462" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_047</v>
-      </c>
-      <c r="N462" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_047</v>
-      </c>
-      <c r="O462" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P462" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q462" s="2">
-        <v>4</v>
-      </c>
-      <c r="R462" s="7"/>
-    </row>
-    <row r="463" spans="1:18">
-      <c r="A463" s="7" t="s">
-        <v>518</v>
-      </c>
-      <c r="B463" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C463" s="2">
-        <v>480</v>
-      </c>
-      <c r="D463" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E463" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_048N@</v>
-      </c>
-      <c r="F463" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_048D@</v>
-      </c>
-      <c r="G463" s="5">
-        <v>480</v>
-      </c>
-      <c r="H463" s="8">
-        <v>0</v>
-      </c>
-      <c r="I463" s="8">
-        <v>50</v>
-      </c>
-      <c r="J463" s="7">
-        <v>70</v>
-      </c>
-      <c r="K463" s="7">
-        <v>30</v>
-      </c>
-      <c r="L463" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_048</v>
-      </c>
-      <c r="N463" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_048</v>
-      </c>
-      <c r="O463" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P463" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q463" s="2">
-        <v>4</v>
-      </c>
-      <c r="R463" s="7"/>
-    </row>
-    <row r="464" spans="1:18">
-      <c r="A464" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="B464" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C464" s="7">
-        <v>490</v>
-      </c>
-      <c r="D464" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E464" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_049N@</v>
-      </c>
-      <c r="F464" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_049D@</v>
-      </c>
-      <c r="G464" s="8">
-        <v>490</v>
-      </c>
-      <c r="H464" s="8">
-        <v>0</v>
-      </c>
-      <c r="I464" s="8">
-        <v>50</v>
-      </c>
-      <c r="J464" s="7">
-        <v>70</v>
-      </c>
-      <c r="K464" s="7">
-        <v>30</v>
-      </c>
-      <c r="L464" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_049</v>
-      </c>
-      <c r="N464" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_049</v>
-      </c>
-      <c r="O464" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P464" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q464" s="2">
-        <v>4</v>
-      </c>
-      <c r="R464" s="7"/>
-    </row>
-    <row r="465" spans="1:18">
-      <c r="A465" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="B465" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C465" s="2">
-        <v>500</v>
-      </c>
-      <c r="D465" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E465" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_050N@</v>
-      </c>
-      <c r="F465" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_050D@</v>
-      </c>
-      <c r="G465" s="5">
-        <v>500</v>
-      </c>
-      <c r="H465" s="8">
-        <v>0</v>
-      </c>
-      <c r="I465" s="8">
-        <v>50</v>
-      </c>
-      <c r="J465" s="7">
-        <v>70</v>
-      </c>
-      <c r="K465" s="7">
-        <v>30</v>
-      </c>
-      <c r="L465" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_050</v>
-      </c>
-      <c r="N465" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_050</v>
-      </c>
-      <c r="O465" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P465" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q465" s="2">
-        <v>4</v>
-      </c>
-      <c r="R465" s="7"/>
-    </row>
-    <row r="466" spans="1:18">
-      <c r="A466" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="B466" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C466" s="7">
-        <v>510</v>
-      </c>
-      <c r="D466" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E466" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_051N@</v>
-      </c>
-      <c r="F466" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_051D@</v>
-      </c>
-      <c r="G466" s="8">
-        <v>510</v>
-      </c>
-      <c r="H466" s="8">
-        <v>0</v>
-      </c>
-      <c r="I466" s="8">
-        <v>50</v>
-      </c>
-      <c r="J466" s="7">
-        <v>70</v>
-      </c>
-      <c r="K466" s="7">
-        <v>30</v>
-      </c>
-      <c r="L466" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_051</v>
-      </c>
-      <c r="N466" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_051</v>
-      </c>
-      <c r="O466" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P466" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q466" s="2">
-        <v>3</v>
-      </c>
-      <c r="R466" s="7"/>
-    </row>
-    <row r="467" spans="1:18">
-      <c r="A467" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="B467" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C467" s="2">
-        <v>520</v>
-      </c>
-      <c r="D467" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E467" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_052N@</v>
-      </c>
-      <c r="F467" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_052D@</v>
-      </c>
-      <c r="G467" s="5">
-        <v>520</v>
-      </c>
-      <c r="H467" s="8">
-        <v>0</v>
-      </c>
-      <c r="I467" s="8">
-        <v>50</v>
-      </c>
-      <c r="J467" s="7">
-        <v>70</v>
-      </c>
-      <c r="K467" s="7">
-        <v>30</v>
-      </c>
-      <c r="L467" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_052</v>
-      </c>
-      <c r="N467" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_052</v>
-      </c>
-      <c r="O467" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P467" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q467" s="2">
-        <v>3</v>
-      </c>
-      <c r="R467" s="7"/>
-    </row>
-    <row r="468" spans="1:18">
-      <c r="A468" s="7" t="s">
-        <v>523</v>
-      </c>
-      <c r="B468" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C468" s="7">
-        <v>530</v>
-      </c>
-      <c r="D468" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E468" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_053N@</v>
-      </c>
-      <c r="F468" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_053D@</v>
-      </c>
-      <c r="G468" s="8">
-        <v>530</v>
-      </c>
-      <c r="H468" s="8">
-        <v>0</v>
-      </c>
-      <c r="I468" s="8">
-        <v>50</v>
-      </c>
-      <c r="J468" s="7">
-        <v>70</v>
-      </c>
-      <c r="K468" s="7">
-        <v>30</v>
-      </c>
-      <c r="L468" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_053</v>
-      </c>
-      <c r="N468" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_053</v>
-      </c>
-      <c r="O468" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P468" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q468" s="2">
-        <v>3</v>
-      </c>
-      <c r="R468" s="7"/>
-    </row>
-    <row r="469" spans="1:18">
-      <c r="A469" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="B469" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C469" s="2">
-        <v>540</v>
-      </c>
-      <c r="D469" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E469" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_054N@</v>
-      </c>
-      <c r="F469" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_054D@</v>
-      </c>
-      <c r="G469" s="5">
-        <v>540</v>
-      </c>
-      <c r="H469" s="8">
-        <v>0</v>
-      </c>
-      <c r="I469" s="8">
-        <v>50</v>
-      </c>
-      <c r="J469" s="7">
-        <v>70</v>
-      </c>
-      <c r="K469" s="7">
-        <v>30</v>
-      </c>
-      <c r="L469" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_054</v>
-      </c>
-      <c r="N469" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_054</v>
-      </c>
-      <c r="O469" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P469" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q469" s="2">
-        <v>4</v>
-      </c>
-      <c r="R469" s="7"/>
-    </row>
-    <row r="470" spans="1:18">
-      <c r="A470" s="7" t="s">
-        <v>525</v>
-      </c>
-      <c r="B470" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C470" s="7">
-        <v>550</v>
-      </c>
-      <c r="D470" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E470" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_055N@</v>
-      </c>
-      <c r="F470" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_055D@</v>
-      </c>
-      <c r="G470" s="8">
-        <v>550</v>
-      </c>
-      <c r="H470" s="8">
-        <v>0</v>
-      </c>
-      <c r="I470" s="8">
-        <v>50</v>
-      </c>
-      <c r="J470" s="7">
-        <v>70</v>
-      </c>
-      <c r="K470" s="7">
-        <v>30</v>
-      </c>
-      <c r="L470" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_055</v>
-      </c>
-      <c r="N470" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_055</v>
-      </c>
-      <c r="O470" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P470" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q470" s="2">
-        <v>4</v>
-      </c>
-      <c r="R470" s="7"/>
-    </row>
-    <row r="471" spans="1:18">
-      <c r="A471" s="7" t="s">
-        <v>526</v>
-      </c>
-      <c r="B471" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C471" s="2">
-        <v>560</v>
-      </c>
-      <c r="D471" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E471" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_056N@</v>
-      </c>
-      <c r="F471" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_056D@</v>
-      </c>
-      <c r="G471" s="5">
-        <v>560</v>
-      </c>
-      <c r="H471" s="8">
-        <v>0</v>
-      </c>
-      <c r="I471" s="8">
-        <v>50</v>
-      </c>
-      <c r="J471" s="7">
-        <v>70</v>
-      </c>
-      <c r="K471" s="7">
-        <v>30</v>
-      </c>
-      <c r="L471" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_056</v>
-      </c>
-      <c r="N471" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_056</v>
-      </c>
-      <c r="O471" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P471" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q471" s="2">
-        <v>4</v>
-      </c>
-      <c r="R471" s="7"/>
-    </row>
-    <row r="472" spans="1:18">
-      <c r="A472" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="B472" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C472" s="7">
-        <v>570</v>
-      </c>
-      <c r="D472" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E472" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_057N@</v>
-      </c>
-      <c r="F472" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_057D@</v>
-      </c>
-      <c r="G472" s="8">
-        <v>570</v>
-      </c>
-      <c r="H472" s="8">
-        <v>0</v>
-      </c>
-      <c r="I472" s="8">
-        <v>50</v>
-      </c>
-      <c r="J472" s="7">
-        <v>70</v>
-      </c>
-      <c r="K472" s="7">
-        <v>30</v>
-      </c>
-      <c r="L472" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_057</v>
-      </c>
-      <c r="N472" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_057</v>
-      </c>
-      <c r="O472" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P472" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q472" s="2">
-        <v>4</v>
-      </c>
-      <c r="R472" s="7"/>
-    </row>
-    <row r="473" spans="1:18">
-      <c r="A473" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="B473" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C473" s="2">
-        <v>580</v>
-      </c>
-      <c r="D473" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E473" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_058N@</v>
-      </c>
-      <c r="F473" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_058D@</v>
-      </c>
-      <c r="G473" s="5">
-        <v>580</v>
-      </c>
-      <c r="H473" s="8">
-        <v>0</v>
-      </c>
-      <c r="I473" s="8">
-        <v>50</v>
-      </c>
-      <c r="J473" s="7">
-        <v>70</v>
-      </c>
-      <c r="K473" s="7">
-        <v>30</v>
-      </c>
-      <c r="L473" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_058</v>
-      </c>
-      <c r="N473" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_058</v>
-      </c>
-      <c r="O473" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P473" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q473" s="2">
-        <v>4</v>
-      </c>
-      <c r="R473" s="7"/>
-    </row>
-    <row r="474" spans="1:18">
-      <c r="A474" s="7" t="s">
-        <v>529</v>
-      </c>
-      <c r="B474" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C474" s="7">
-        <v>590</v>
-      </c>
-      <c r="D474" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E474" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_059N@</v>
-      </c>
-      <c r="F474" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_059D@</v>
-      </c>
-      <c r="G474" s="8">
-        <v>590</v>
-      </c>
-      <c r="H474" s="8">
-        <v>0</v>
-      </c>
-      <c r="I474" s="8">
-        <v>50</v>
-      </c>
-      <c r="J474" s="7">
-        <v>70</v>
-      </c>
-      <c r="K474" s="7">
-        <v>30</v>
-      </c>
-      <c r="L474" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_059</v>
-      </c>
-      <c r="N474" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_059</v>
-      </c>
-      <c r="O474" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P474" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q474" s="2">
-        <v>4</v>
-      </c>
-      <c r="R474" s="7"/>
-    </row>
-    <row r="475" spans="1:18">
-      <c r="A475" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="B475" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C475" s="2">
-        <v>600</v>
-      </c>
-      <c r="D475" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E475" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_060N@</v>
-      </c>
-      <c r="F475" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_060D@</v>
-      </c>
-      <c r="G475" s="5">
-        <v>600</v>
-      </c>
-      <c r="H475" s="8">
-        <v>0</v>
-      </c>
-      <c r="I475" s="8">
-        <v>50</v>
-      </c>
-      <c r="J475" s="7">
-        <v>70</v>
-      </c>
-      <c r="K475" s="7">
-        <v>30</v>
-      </c>
-      <c r="L475" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_060</v>
-      </c>
-      <c r="N475" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_060</v>
-      </c>
-      <c r="O475" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P475" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q475" s="2">
-        <v>4</v>
-      </c>
-      <c r="R475" s="7"/>
-    </row>
-    <row r="476" spans="1:18">
-      <c r="A476" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="B476" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C476" s="7">
-        <v>610</v>
-      </c>
-      <c r="D476" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E476" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_061N@</v>
-      </c>
-      <c r="F476" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_061D@</v>
-      </c>
-      <c r="G476" s="8">
-        <v>610</v>
-      </c>
-      <c r="H476" s="8">
-        <v>0</v>
-      </c>
-      <c r="I476" s="8">
-        <v>50</v>
-      </c>
-      <c r="J476" s="7">
-        <v>70</v>
-      </c>
-      <c r="K476" s="7">
-        <v>30</v>
-      </c>
-      <c r="L476" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_061</v>
-      </c>
-      <c r="N476" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_061</v>
-      </c>
-      <c r="O476" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P476" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q476" s="2">
-        <v>4</v>
-      </c>
-      <c r="R476" s="7"/>
-    </row>
-    <row r="477" spans="1:18">
-      <c r="A477" s="7" t="s">
-        <v>532</v>
-      </c>
-      <c r="B477" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C477" s="2">
-        <v>620</v>
-      </c>
-      <c r="D477" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E477" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_062N@</v>
-      </c>
-      <c r="F477" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_062D@</v>
-      </c>
-      <c r="G477" s="5">
-        <v>620</v>
-      </c>
-      <c r="H477" s="8">
-        <v>0</v>
-      </c>
-      <c r="I477" s="8">
-        <v>50</v>
-      </c>
-      <c r="J477" s="7">
-        <v>70</v>
-      </c>
-      <c r="K477" s="7">
-        <v>30</v>
-      </c>
-      <c r="L477" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_062</v>
-      </c>
-      <c r="N477" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_062</v>
-      </c>
-      <c r="O477" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P477" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q477" s="2">
-        <v>4</v>
-      </c>
-      <c r="R477" s="7"/>
-    </row>
-    <row r="478" spans="1:18">
-      <c r="A478" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="B478" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C478" s="7">
-        <v>630</v>
-      </c>
-      <c r="D478" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E478" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_063N@</v>
-      </c>
-      <c r="F478" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_063D@</v>
-      </c>
-      <c r="G478" s="8">
-        <v>630</v>
-      </c>
-      <c r="H478" s="8">
-        <v>0</v>
-      </c>
-      <c r="I478" s="8">
-        <v>50</v>
-      </c>
-      <c r="J478" s="7">
-        <v>70</v>
-      </c>
-      <c r="K478" s="7">
-        <v>30</v>
-      </c>
-      <c r="L478" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_063</v>
-      </c>
-      <c r="N478" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_063</v>
-      </c>
-      <c r="O478" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P478" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q478" s="2">
-        <v>3</v>
-      </c>
-      <c r="R478" s="7"/>
-    </row>
-    <row r="479" spans="1:18">
-      <c r="A479" s="7" t="s">
-        <v>534</v>
-      </c>
-      <c r="B479" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C479" s="2">
-        <v>640</v>
-      </c>
-      <c r="D479" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E479" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_064N@</v>
-      </c>
-      <c r="F479" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_064D@</v>
-      </c>
-      <c r="G479" s="5">
-        <v>640</v>
-      </c>
-      <c r="H479" s="8">
-        <v>0</v>
-      </c>
-      <c r="I479" s="8">
-        <v>50</v>
-      </c>
-      <c r="J479" s="7">
-        <v>70</v>
-      </c>
-      <c r="K479" s="7">
-        <v>30</v>
-      </c>
-      <c r="L479" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_064</v>
-      </c>
-      <c r="N479" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_064</v>
-      </c>
-      <c r="O479" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P479" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q479" s="2">
-        <v>3</v>
-      </c>
-      <c r="R479" s="7"/>
-    </row>
-    <row r="480" spans="1:18">
-      <c r="A480" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="B480" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C480" s="7">
-        <v>650</v>
-      </c>
-      <c r="D480" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E480" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_065N@</v>
-      </c>
-      <c r="F480" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_065D@</v>
-      </c>
-      <c r="G480" s="8">
-        <v>650</v>
-      </c>
-      <c r="H480" s="8">
-        <v>0</v>
-      </c>
-      <c r="I480" s="8">
-        <v>50</v>
-      </c>
-      <c r="J480" s="7">
-        <v>70</v>
-      </c>
-      <c r="K480" s="7">
-        <v>30</v>
-      </c>
-      <c r="L480" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_065</v>
-      </c>
-      <c r="N480" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_065</v>
-      </c>
-      <c r="O480" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P480" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q480" s="2">
-        <v>3</v>
-      </c>
-      <c r="R480" s="7"/>
-    </row>
-    <row r="481" spans="1:18">
-      <c r="A481" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="B481" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C481" s="2">
-        <v>660</v>
-      </c>
-      <c r="D481" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E481" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_066N@</v>
-      </c>
-      <c r="F481" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_066D@</v>
-      </c>
-      <c r="G481" s="5">
-        <v>660</v>
-      </c>
-      <c r="H481" s="8">
-        <v>0</v>
-      </c>
-      <c r="I481" s="8">
-        <v>50</v>
-      </c>
-      <c r="J481" s="7">
-        <v>70</v>
-      </c>
-      <c r="K481" s="7">
-        <v>30</v>
-      </c>
-      <c r="L481" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_066</v>
-      </c>
-      <c r="N481" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_066</v>
-      </c>
-      <c r="O481" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P481" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q481" s="2">
-        <v>4</v>
-      </c>
-      <c r="R481" s="7"/>
-    </row>
-    <row r="482" spans="1:18">
-      <c r="A482" s="7" t="s">
-        <v>537</v>
-      </c>
-      <c r="B482" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C482" s="7">
-        <v>670</v>
-      </c>
-      <c r="D482" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E482" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_067N@</v>
-      </c>
-      <c r="F482" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_067D@</v>
-      </c>
-      <c r="G482" s="8">
-        <v>670</v>
-      </c>
-      <c r="H482" s="8">
-        <v>0</v>
-      </c>
-      <c r="I482" s="8">
-        <v>50</v>
-      </c>
-      <c r="J482" s="7">
-        <v>70</v>
-      </c>
-      <c r="K482" s="7">
-        <v>30</v>
-      </c>
-      <c r="L482" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_067</v>
-      </c>
-      <c r="N482" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_067</v>
-      </c>
-      <c r="O482" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P482" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q482" s="2">
-        <v>4</v>
-      </c>
-      <c r="R482" s="7"/>
-    </row>
-    <row r="483" spans="1:18">
-      <c r="A483" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="B483" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C483" s="2">
-        <v>680</v>
-      </c>
-      <c r="D483" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E483" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_068N@</v>
-      </c>
-      <c r="F483" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_068D@</v>
-      </c>
-      <c r="G483" s="5">
-        <v>680</v>
-      </c>
-      <c r="H483" s="8">
-        <v>0</v>
-      </c>
-      <c r="I483" s="8">
-        <v>50</v>
-      </c>
-      <c r="J483" s="7">
-        <v>70</v>
-      </c>
-      <c r="K483" s="7">
-        <v>30</v>
-      </c>
-      <c r="L483" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_068</v>
-      </c>
-      <c r="N483" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_068</v>
-      </c>
-      <c r="O483" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P483" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q483" s="2">
-        <v>4</v>
-      </c>
-      <c r="R483" s="7"/>
-    </row>
-    <row r="484" spans="1:18">
-      <c r="A484" s="7" t="s">
-        <v>539</v>
-      </c>
-      <c r="B484" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C484" s="7">
-        <v>690</v>
-      </c>
-      <c r="D484" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E484" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_069N@</v>
-      </c>
-      <c r="F484" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_069D@</v>
-      </c>
-      <c r="G484" s="8">
-        <v>690</v>
-      </c>
-      <c r="H484" s="8">
-        <v>0</v>
-      </c>
-      <c r="I484" s="8">
-        <v>50</v>
-      </c>
-      <c r="J484" s="7">
-        <v>70</v>
-      </c>
-      <c r="K484" s="7">
-        <v>30</v>
-      </c>
-      <c r="L484" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_069</v>
-      </c>
-      <c r="N484" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_069</v>
-      </c>
-      <c r="O484" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P484" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q484" s="2">
-        <v>4</v>
-      </c>
-      <c r="R484" s="7"/>
-    </row>
-    <row r="485" spans="1:18">
-      <c r="A485" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="B485" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C485" s="2">
-        <v>700</v>
-      </c>
-      <c r="D485" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E485" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_070N@</v>
-      </c>
-      <c r="F485" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_070D@</v>
-      </c>
-      <c r="G485" s="5">
-        <v>700</v>
-      </c>
-      <c r="H485" s="8">
-        <v>0</v>
-      </c>
-      <c r="I485" s="8">
-        <v>50</v>
-      </c>
-      <c r="J485" s="7">
-        <v>70</v>
-      </c>
-      <c r="K485" s="7">
-        <v>30</v>
-      </c>
-      <c r="L485" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_070</v>
-      </c>
-      <c r="N485" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_070</v>
-      </c>
-      <c r="O485" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P485" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q485" s="2">
-        <v>4</v>
-      </c>
-      <c r="R485" s="7"/>
-    </row>
-    <row r="486" spans="1:18">
-      <c r="A486" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="B486" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C486" s="7">
-        <v>710</v>
-      </c>
-      <c r="D486" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E486" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_071N@</v>
-      </c>
-      <c r="F486" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_071D@</v>
-      </c>
-      <c r="G486" s="8">
-        <v>710</v>
-      </c>
-      <c r="H486" s="8">
-        <v>0</v>
-      </c>
-      <c r="I486" s="8">
-        <v>50</v>
-      </c>
-      <c r="J486" s="7">
-        <v>70</v>
-      </c>
-      <c r="K486" s="7">
-        <v>30</v>
-      </c>
-      <c r="L486" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_071</v>
-      </c>
-      <c r="N486" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_071</v>
-      </c>
-      <c r="O486" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P486" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q486" s="2">
-        <v>4</v>
-      </c>
-      <c r="R486" s="7"/>
-    </row>
-    <row r="487" spans="1:18">
-      <c r="A487" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="B487" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C487" s="2">
-        <v>720</v>
-      </c>
-      <c r="D487" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E487" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_072N@</v>
-      </c>
-      <c r="F487" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_072D@</v>
-      </c>
-      <c r="G487" s="5">
-        <v>720</v>
-      </c>
-      <c r="H487" s="8">
-        <v>0</v>
-      </c>
-      <c r="I487" s="8">
-        <v>50</v>
-      </c>
-      <c r="J487" s="7">
-        <v>70</v>
-      </c>
-      <c r="K487" s="7">
-        <v>30</v>
-      </c>
-      <c r="L487" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_072</v>
-      </c>
-      <c r="N487" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_072</v>
-      </c>
-      <c r="O487" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P487" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q487" s="2">
-        <v>4</v>
-      </c>
-      <c r="R487" s="7"/>
-    </row>
-    <row r="488" spans="1:18">
-      <c r="A488" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="B488" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C488" s="7">
-        <v>730</v>
-      </c>
-      <c r="D488" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E488" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_073N@</v>
-      </c>
-      <c r="F488" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_073D@</v>
-      </c>
-      <c r="G488" s="8">
-        <v>730</v>
-      </c>
-      <c r="H488" s="8">
-        <v>0</v>
-      </c>
-      <c r="I488" s="8">
-        <v>50</v>
-      </c>
-      <c r="J488" s="7">
-        <v>70</v>
-      </c>
-      <c r="K488" s="7">
-        <v>30</v>
-      </c>
-      <c r="L488" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_073</v>
-      </c>
-      <c r="N488" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_073</v>
-      </c>
-      <c r="O488" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P488" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q488" s="2">
-        <v>4</v>
-      </c>
-      <c r="R488" s="7"/>
-    </row>
-    <row r="489" spans="1:18">
-      <c r="A489" s="7" t="s">
-        <v>544</v>
-      </c>
-      <c r="B489" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C489" s="2">
-        <v>740</v>
-      </c>
-      <c r="D489" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E489" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_074N@</v>
-      </c>
-      <c r="F489" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_074D@</v>
-      </c>
-      <c r="G489" s="5">
-        <v>740</v>
-      </c>
-      <c r="H489" s="8">
-        <v>0</v>
-      </c>
-      <c r="I489" s="8">
-        <v>50</v>
-      </c>
-      <c r="J489" s="7">
-        <v>70</v>
-      </c>
-      <c r="K489" s="7">
-        <v>30</v>
-      </c>
-      <c r="L489" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_074</v>
-      </c>
-      <c r="N489" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_074</v>
-      </c>
-      <c r="O489" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P489" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q489" s="2">
-        <v>4</v>
-      </c>
-      <c r="R489" s="7"/>
-    </row>
-    <row r="490" spans="1:18">
-      <c r="A490" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="B490" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C490" s="7">
-        <v>750</v>
-      </c>
-      <c r="D490" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E490" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_075N@</v>
-      </c>
-      <c r="F490" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_075D@</v>
-      </c>
-      <c r="G490" s="8">
-        <v>750</v>
-      </c>
-      <c r="H490" s="8">
-        <v>0</v>
-      </c>
-      <c r="I490" s="8">
-        <v>50</v>
-      </c>
-      <c r="J490" s="7">
-        <v>70</v>
-      </c>
-      <c r="K490" s="7">
-        <v>30</v>
-      </c>
-      <c r="L490" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_075</v>
-      </c>
-      <c r="N490" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_075</v>
-      </c>
-      <c r="O490" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P490" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q490" s="2">
-        <v>4</v>
-      </c>
-      <c r="R490" s="7"/>
-    </row>
-    <row r="491" spans="1:18">
-      <c r="A491" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="B491" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C491" s="2">
-        <v>760</v>
-      </c>
-      <c r="D491" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E491" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_076N@</v>
-      </c>
-      <c r="F491" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_076D@</v>
-      </c>
-      <c r="G491" s="5">
-        <v>760</v>
-      </c>
-      <c r="H491" s="8">
-        <v>0</v>
-      </c>
-      <c r="I491" s="8">
-        <v>50</v>
-      </c>
-      <c r="J491" s="7">
-        <v>70</v>
-      </c>
-      <c r="K491" s="7">
-        <v>30</v>
-      </c>
-      <c r="L491" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_076</v>
-      </c>
-      <c r="N491" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_076</v>
-      </c>
-      <c r="O491" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P491" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q491" s="2">
-        <v>3</v>
-      </c>
-      <c r="R491" s="7"/>
-    </row>
-    <row r="492" spans="1:18">
-      <c r="A492" s="7" t="s">
-        <v>547</v>
-      </c>
-      <c r="B492" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C492" s="7">
-        <v>770</v>
-      </c>
-      <c r="D492" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E492" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_077N@</v>
-      </c>
-      <c r="F492" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_077D@</v>
-      </c>
-      <c r="G492" s="8">
-        <v>770</v>
-      </c>
-      <c r="H492" s="8">
-        <v>0</v>
-      </c>
-      <c r="I492" s="8">
-        <v>50</v>
-      </c>
-      <c r="J492" s="7">
-        <v>70</v>
-      </c>
-      <c r="K492" s="7">
-        <v>30</v>
-      </c>
-      <c r="L492" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_077</v>
-      </c>
-      <c r="N492" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_077</v>
-      </c>
-      <c r="O492" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P492" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q492" s="2">
-        <v>3</v>
-      </c>
-      <c r="R492" s="7"/>
-    </row>
-    <row r="493" spans="1:18">
-      <c r="A493" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="B493" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C493" s="2">
-        <v>780</v>
-      </c>
-      <c r="D493" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E493" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_078N@</v>
-      </c>
-      <c r="F493" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_078D@</v>
-      </c>
-      <c r="G493" s="5">
-        <v>780</v>
-      </c>
-      <c r="H493" s="8">
-        <v>0</v>
-      </c>
-      <c r="I493" s="8">
-        <v>50</v>
-      </c>
-      <c r="J493" s="7">
-        <v>70</v>
-      </c>
-      <c r="K493" s="7">
-        <v>30</v>
-      </c>
-      <c r="L493" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_078</v>
-      </c>
-      <c r="N493" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_078</v>
-      </c>
-      <c r="O493" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P493" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q493" s="2">
-        <v>3</v>
-      </c>
-      <c r="R493" s="7"/>
-    </row>
-    <row r="494" spans="1:18">
-      <c r="A494" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="B494" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C494" s="7">
-        <v>790</v>
-      </c>
-      <c r="D494" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E494" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_079N@</v>
-      </c>
-      <c r="F494" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_079D@</v>
-      </c>
-      <c r="G494" s="8">
-        <v>790</v>
-      </c>
-      <c r="H494" s="8">
-        <v>0</v>
-      </c>
-      <c r="I494" s="8">
-        <v>50</v>
-      </c>
-      <c r="J494" s="7">
-        <v>70</v>
-      </c>
-      <c r="K494" s="7">
-        <v>30</v>
-      </c>
-      <c r="L494" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_079</v>
-      </c>
-      <c r="N494" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_079</v>
-      </c>
-      <c r="O494" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P494" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q494" s="2">
-        <v>4</v>
-      </c>
-      <c r="R494" s="7"/>
-    </row>
-    <row r="495" spans="1:18">
-      <c r="A495" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="B495" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C495" s="2">
-        <v>800</v>
-      </c>
-      <c r="D495" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E495" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_080N@</v>
-      </c>
-      <c r="F495" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_080D@</v>
-      </c>
-      <c r="G495" s="5">
-        <v>800</v>
-      </c>
-      <c r="H495" s="8">
-        <v>0</v>
-      </c>
-      <c r="I495" s="8">
-        <v>50</v>
-      </c>
-      <c r="J495" s="7">
-        <v>70</v>
-      </c>
-      <c r="K495" s="7">
-        <v>30</v>
-      </c>
-      <c r="L495" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_080</v>
-      </c>
-      <c r="N495" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_080</v>
-      </c>
-      <c r="O495" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P495" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q495" s="2">
-        <v>4</v>
-      </c>
-      <c r="R495" s="7"/>
-    </row>
-    <row r="496" spans="1:18">
-      <c r="A496" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="B496" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C496" s="7">
-        <v>810</v>
-      </c>
-      <c r="D496" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E496" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_081N@</v>
-      </c>
-      <c r="F496" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_081D@</v>
-      </c>
-      <c r="G496" s="8">
-        <v>810</v>
-      </c>
-      <c r="H496" s="8">
-        <v>0</v>
-      </c>
-      <c r="I496" s="8">
-        <v>50</v>
-      </c>
-      <c r="J496" s="7">
-        <v>70</v>
-      </c>
-      <c r="K496" s="7">
-        <v>30</v>
-      </c>
-      <c r="L496" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_081</v>
-      </c>
-      <c r="N496" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_081</v>
-      </c>
-      <c r="O496" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P496" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q496" s="2">
-        <v>4</v>
-      </c>
-      <c r="R496" s="7"/>
-    </row>
-    <row r="497" spans="1:18">
-      <c r="A497" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="B497" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C497" s="2">
-        <v>820</v>
-      </c>
-      <c r="D497" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E497" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_082N@</v>
-      </c>
-      <c r="F497" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_082D@</v>
-      </c>
-      <c r="G497" s="5">
-        <v>820</v>
-      </c>
-      <c r="H497" s="8">
-        <v>0</v>
-      </c>
-      <c r="I497" s="8">
-        <v>50</v>
-      </c>
-      <c r="J497" s="7">
-        <v>70</v>
-      </c>
-      <c r="K497" s="7">
-        <v>30</v>
-      </c>
-      <c r="L497" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_082</v>
-      </c>
-      <c r="N497" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_082</v>
-      </c>
-      <c r="O497" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P497" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q497" s="2">
-        <v>4</v>
-      </c>
-      <c r="R497" s="7"/>
-    </row>
-    <row r="498" spans="1:18">
-      <c r="A498" s="7" t="s">
-        <v>553</v>
-      </c>
-      <c r="B498" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C498" s="7">
-        <v>830</v>
-      </c>
-      <c r="D498" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E498" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_083N@</v>
-      </c>
-      <c r="F498" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_083D@</v>
-      </c>
-      <c r="G498" s="8">
-        <v>830</v>
-      </c>
-      <c r="H498" s="8">
-        <v>0</v>
-      </c>
-      <c r="I498" s="8">
-        <v>50</v>
-      </c>
-      <c r="J498" s="7">
-        <v>70</v>
-      </c>
-      <c r="K498" s="7">
-        <v>30</v>
-      </c>
-      <c r="L498" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_083</v>
-      </c>
-      <c r="N498" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_083</v>
-      </c>
-      <c r="O498" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P498" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q498" s="2">
-        <v>4</v>
-      </c>
-      <c r="R498" s="7"/>
-    </row>
-    <row r="499" spans="1:18">
-      <c r="A499" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="B499" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C499" s="2">
-        <v>840</v>
-      </c>
-      <c r="D499" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E499" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_084N@</v>
-      </c>
-      <c r="F499" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_084D@</v>
-      </c>
-      <c r="G499" s="5">
-        <v>840</v>
-      </c>
-      <c r="H499" s="8">
-        <v>0</v>
-      </c>
-      <c r="I499" s="8">
-        <v>50</v>
-      </c>
-      <c r="J499" s="7">
-        <v>70</v>
-      </c>
-      <c r="K499" s="7">
-        <v>30</v>
-      </c>
-      <c r="L499" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_084</v>
-      </c>
-      <c r="N499" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_084</v>
-      </c>
-      <c r="O499" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P499" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q499" s="2">
-        <v>4</v>
-      </c>
-      <c r="R499" s="7"/>
-    </row>
-    <row r="500" spans="1:18">
-      <c r="A500" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="B500" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C500" s="7">
-        <v>850</v>
-      </c>
-      <c r="D500" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E500" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_085N@</v>
-      </c>
-      <c r="F500" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_085D@</v>
-      </c>
-      <c r="G500" s="8">
-        <v>850</v>
-      </c>
-      <c r="H500" s="8">
-        <v>0</v>
-      </c>
-      <c r="I500" s="8">
-        <v>50</v>
-      </c>
-      <c r="J500" s="7">
-        <v>70</v>
-      </c>
-      <c r="K500" s="7">
-        <v>30</v>
-      </c>
-      <c r="L500" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_085</v>
-      </c>
-      <c r="N500" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_085</v>
-      </c>
-      <c r="O500" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P500" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q500" s="2">
-        <v>4</v>
-      </c>
-      <c r="R500" s="7"/>
-    </row>
-    <row r="501" spans="1:18">
-      <c r="A501" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="B501" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C501" s="2">
-        <v>860</v>
-      </c>
-      <c r="D501" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E501" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_086N@</v>
-      </c>
-      <c r="F501" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_086D@</v>
-      </c>
-      <c r="G501" s="5">
-        <v>860</v>
-      </c>
-      <c r="H501" s="8">
-        <v>0</v>
-      </c>
-      <c r="I501" s="8">
-        <v>50</v>
-      </c>
-      <c r="J501" s="7">
-        <v>70</v>
-      </c>
-      <c r="K501" s="7">
-        <v>30</v>
-      </c>
-      <c r="L501" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_086</v>
-      </c>
-      <c r="N501" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_086</v>
-      </c>
-      <c r="O501" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P501" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q501" s="2">
-        <v>4</v>
-      </c>
-      <c r="R501" s="7"/>
-    </row>
-    <row r="502" spans="1:18">
-      <c r="A502" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="B502" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C502" s="7">
-        <v>870</v>
-      </c>
-      <c r="D502" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E502" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_087N@</v>
-      </c>
-      <c r="F502" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_087D@</v>
-      </c>
-      <c r="G502" s="8">
-        <v>870</v>
-      </c>
-      <c r="H502" s="8">
-        <v>0</v>
-      </c>
-      <c r="I502" s="8">
-        <v>50</v>
-      </c>
-      <c r="J502" s="7">
-        <v>70</v>
-      </c>
-      <c r="K502" s="7">
-        <v>30</v>
-      </c>
-      <c r="L502" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_087</v>
-      </c>
-      <c r="N502" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_087</v>
-      </c>
-      <c r="O502" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P502" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q502" s="2">
-        <v>4</v>
-      </c>
-      <c r="R502" s="7"/>
-    </row>
-    <row r="503" spans="1:18">
-      <c r="A503" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="B503" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C503" s="2">
-        <v>880</v>
-      </c>
-      <c r="D503" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E503" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_088N@</v>
-      </c>
-      <c r="F503" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_088D@</v>
-      </c>
-      <c r="G503" s="5">
-        <v>880</v>
-      </c>
-      <c r="H503" s="8">
-        <v>0</v>
-      </c>
-      <c r="I503" s="8">
-        <v>50</v>
-      </c>
-      <c r="J503" s="7">
-        <v>70</v>
-      </c>
-      <c r="K503" s="7">
-        <v>30</v>
-      </c>
-      <c r="L503" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_088</v>
-      </c>
-      <c r="N503" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_088</v>
-      </c>
-      <c r="O503" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P503" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q503" s="2">
-        <v>3</v>
-      </c>
-      <c r="R503" s="7"/>
-    </row>
-    <row r="504" spans="1:18">
-      <c r="A504" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="B504" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C504" s="7">
-        <v>890</v>
-      </c>
-      <c r="D504" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E504" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_089N@</v>
-      </c>
-      <c r="F504" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_089D@</v>
-      </c>
-      <c r="G504" s="8">
-        <v>890</v>
-      </c>
-      <c r="H504" s="8">
-        <v>0</v>
-      </c>
-      <c r="I504" s="8">
-        <v>50</v>
-      </c>
-      <c r="J504" s="7">
-        <v>70</v>
-      </c>
-      <c r="K504" s="7">
-        <v>30</v>
-      </c>
-      <c r="L504" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_089</v>
-      </c>
-      <c r="N504" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_089</v>
-      </c>
-      <c r="O504" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P504" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q504" s="2">
-        <v>3</v>
-      </c>
-      <c r="R504" s="7"/>
-    </row>
-    <row r="505" spans="1:18">
-      <c r="A505" s="7" t="s">
-        <v>560</v>
-      </c>
-      <c r="B505" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C505" s="2">
-        <v>900</v>
-      </c>
-      <c r="D505" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="E505" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
-        <v>@SR00_090N@</v>
-      </c>
-      <c r="F505" s="7" t="str">
-        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
-        <v>@SR00_090D@</v>
-      </c>
-      <c r="G505" s="5">
-        <v>900</v>
-      </c>
-      <c r="H505" s="8">
-        <v>0</v>
-      </c>
-      <c r="I505" s="8">
-        <v>50</v>
-      </c>
-      <c r="J505" s="7">
-        <v>70</v>
-      </c>
-      <c r="K505" s="7">
-        <v>30</v>
-      </c>
-      <c r="L505" s="7" t="str">
-        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
-        <v>BR00_090</v>
-      </c>
-      <c r="N505" s="7" t="str">
-        <f>표28[[#This Row],[groupid]]</f>
-        <v>BR00_090</v>
-      </c>
-      <c r="O505" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P505" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q505" s="2">
-        <v>3</v>
-      </c>
-      <c r="R505" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -30236,7 +27590,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -30274,8 +27628,8 @@
       <c r="C2">
         <v>5200</v>
       </c>
-      <c r="D2" s="9">
-        <v>6.4396000000000004</v>
+      <c r="D2">
+        <v>3.3361999999999998</v>
       </c>
       <c r="E2">
         <v>86</v>
@@ -30291,8 +27645,8 @@
       <c r="C3">
         <v>5300</v>
       </c>
-      <c r="D3" s="10">
-        <v>53.220199999999998</v>
+      <c r="D3">
+        <v>36.895000000000003</v>
       </c>
       <c r="E3">
         <v>2001</v>
@@ -30308,8 +27662,8 @@
       <c r="C4">
         <v>5500</v>
       </c>
-      <c r="D4" s="11">
-        <v>1301.57</v>
+      <c r="D4" s="4">
+        <v>1017.7</v>
       </c>
       <c r="E4">
         <v>108544.00000000048</v>
@@ -30325,8 +27679,8 @@
       <c r="C5">
         <v>5700</v>
       </c>
-      <c r="D5" s="12">
-        <v>47625</v>
+      <c r="D5">
+        <v>39766</v>
       </c>
       <c r="E5">
         <v>7733248</v>
@@ -30342,8 +27696,8 @@
       <c r="C6">
         <v>6100</v>
       </c>
-      <c r="D6" s="13">
-        <v>17892498</v>
+      <c r="D6">
+        <v>15589731</v>
       </c>
       <c r="E6">
         <v>6056866302</v>
@@ -30359,8 +27713,8 @@
       <c r="C7">
         <v>6300</v>
       </c>
-      <c r="D7" s="14">
-        <v>5564051276</v>
+      <c r="D7">
+        <v>4990733267</v>
       </c>
       <c r="E7">
         <v>3509157065962</v>
@@ -30376,8 +27730,8 @@
       <c r="C8">
         <v>6700</v>
       </c>
-      <c r="D8" s="15">
-        <v>1831700929713</v>
+      <c r="D8">
+        <v>1677322427419</v>
       </c>
       <c r="E8">
         <v>2005605675653396</v>
@@ -30393,8 +27747,8 @@
       <c r="C9">
         <v>6900</v>
       </c>
-      <c r="D9" s="16">
-        <v>1411744908409495.7</v>
+      <c r="D9">
+        <v>1312779264637361.5</v>
       </c>
       <c r="E9">
         <v>2.6376361699820129E+18</v>
@@ -30410,7 +27764,7 @@
       <c r="C10">
         <v>7300</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="4">
         <v>1.9356116650602877E+18</v>
       </c>
       <c r="E10">

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "리서치 시스템 완료 ㅠㅠ""""
This reverts commit e5d6ac39537060ff278e1030703289396381b9eb.
</commit_message>
<xml_diff>
--- a/Doc/XmlDataDocument.xlsx
+++ b/Doc/XmlDataDocument.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2569" uniqueCount="561">
   <si>
     <t>R01</t>
   </si>
@@ -1651,6 +1651,141 @@
   <si>
     <t>DpcX</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R00_046</t>
+  </si>
+  <si>
+    <t>R00_047</t>
+  </si>
+  <si>
+    <t>R00_048</t>
+  </si>
+  <si>
+    <t>R00_049</t>
+  </si>
+  <si>
+    <t>R00_050</t>
+  </si>
+  <si>
+    <t>R00_051</t>
+  </si>
+  <si>
+    <t>R00_052</t>
+  </si>
+  <si>
+    <t>R00_053</t>
+  </si>
+  <si>
+    <t>R00_054</t>
+  </si>
+  <si>
+    <t>R00_055</t>
+  </si>
+  <si>
+    <t>R00_056</t>
+  </si>
+  <si>
+    <t>R00_057</t>
+  </si>
+  <si>
+    <t>R00_058</t>
+  </si>
+  <si>
+    <t>R00_059</t>
+  </si>
+  <si>
+    <t>R00_060</t>
+  </si>
+  <si>
+    <t>R00_061</t>
+  </si>
+  <si>
+    <t>R00_062</t>
+  </si>
+  <si>
+    <t>R00_063</t>
+  </si>
+  <si>
+    <t>R00_064</t>
+  </si>
+  <si>
+    <t>R00_065</t>
+  </si>
+  <si>
+    <t>R00_066</t>
+  </si>
+  <si>
+    <t>R00_067</t>
+  </si>
+  <si>
+    <t>R00_068</t>
+  </si>
+  <si>
+    <t>R00_069</t>
+  </si>
+  <si>
+    <t>R00_070</t>
+  </si>
+  <si>
+    <t>R00_071</t>
+  </si>
+  <si>
+    <t>R00_072</t>
+  </si>
+  <si>
+    <t>R00_073</t>
+  </si>
+  <si>
+    <t>R00_074</t>
+  </si>
+  <si>
+    <t>R00_075</t>
+  </si>
+  <si>
+    <t>R00_076</t>
+  </si>
+  <si>
+    <t>R00_077</t>
+  </si>
+  <si>
+    <t>R00_078</t>
+  </si>
+  <si>
+    <t>R00_079</t>
+  </si>
+  <si>
+    <t>R00_080</t>
+  </si>
+  <si>
+    <t>R00_081</t>
+  </si>
+  <si>
+    <t>R00_082</t>
+  </si>
+  <si>
+    <t>R00_083</t>
+  </si>
+  <si>
+    <t>R00_084</t>
+  </si>
+  <si>
+    <t>R00_085</t>
+  </si>
+  <si>
+    <t>R00_086</t>
+  </si>
+  <si>
+    <t>R00_087</t>
+  </si>
+  <si>
+    <t>R00_088</t>
+  </si>
+  <si>
+    <t>R00_089</t>
+  </si>
+  <si>
+    <t>R00_090</t>
   </si>
 </sst>
 </file>
@@ -1682,12 +1817,18 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1704,7 +1845,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1730,6 +1871,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1905,8 +2073,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="표28" displayName="표28" ref="A1:L460" tableType="xml" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" connectionId="8">
-  <autoFilter ref="A1:L460">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="표28" displayName="표28" ref="A1:L505" tableType="xml" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" connectionId="8">
+  <autoFilter ref="A1:L505">
     <filterColumn colId="8"/>
     <filterColumn colId="10"/>
     <filterColumn colId="11"/>
@@ -1955,8 +2123,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="표29" displayName="표29" ref="N1:R460" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="2">
-  <autoFilter ref="N1:R460"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="표29" displayName="표29" ref="N1:R505" tableType="xml" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" connectionId="2">
+  <autoFilter ref="N1:R505"/>
   <tableColumns count="5">
     <tableColumn id="1" uniqueName="group" name="group" dataDxfId="4">
       <calculatedColumnFormula>표28[[#This Row],[groupid]]</calculatedColumnFormula>
@@ -2288,10 +2456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R460"/>
+  <dimension ref="A1:R505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A411" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J428" sqref="J428"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2401,7 +2572,7 @@
         <v>70</v>
       </c>
       <c r="K2" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2455,7 +2626,7 @@
         <v>70</v>
       </c>
       <c r="K3" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2509,7 +2680,7 @@
         <v>70</v>
       </c>
       <c r="K4" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2563,7 +2734,7 @@
         <v>70</v>
       </c>
       <c r="K5" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L5" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2617,7 +2788,7 @@
         <v>70</v>
       </c>
       <c r="K6" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L6" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2671,7 +2842,7 @@
         <v>70</v>
       </c>
       <c r="K7" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L7" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2725,7 +2896,7 @@
         <v>70</v>
       </c>
       <c r="K8" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2779,7 +2950,7 @@
         <v>70</v>
       </c>
       <c r="K9" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2833,7 +3004,7 @@
         <v>70</v>
       </c>
       <c r="K10" s="2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="L10" s="1" t="str">
         <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
@@ -2959,7 +3130,7 @@
         <v>101</v>
       </c>
       <c r="Q12" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -3013,7 +3184,7 @@
         <v>101</v>
       </c>
       <c r="Q13" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -3067,7 +3238,7 @@
         <v>101</v>
       </c>
       <c r="Q14" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -3121,7 +3292,7 @@
         <v>101</v>
       </c>
       <c r="Q15" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -3445,7 +3616,7 @@
         <v>101</v>
       </c>
       <c r="Q21" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -3499,7 +3670,7 @@
         <v>101</v>
       </c>
       <c r="Q22" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -3553,7 +3724,7 @@
         <v>101</v>
       </c>
       <c r="Q23" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -3607,7 +3778,7 @@
         <v>101</v>
       </c>
       <c r="Q24" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -3661,7 +3832,7 @@
         <v>101</v>
       </c>
       <c r="Q25" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -3715,7 +3886,7 @@
         <v>101</v>
       </c>
       <c r="Q26" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -3769,7 +3940,7 @@
         <v>101</v>
       </c>
       <c r="Q27" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -3823,7 +3994,7 @@
         <v>101</v>
       </c>
       <c r="Q28" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -3877,7 +4048,7 @@
         <v>101</v>
       </c>
       <c r="Q29" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -3931,7 +4102,7 @@
         <v>101</v>
       </c>
       <c r="Q30" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -3985,7 +4156,7 @@
         <v>101</v>
       </c>
       <c r="Q31" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -4201,7 +4372,7 @@
         <v>101</v>
       </c>
       <c r="Q35" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -4363,7 +4534,7 @@
         <v>101</v>
       </c>
       <c r="Q38" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -4417,7 +4588,7 @@
         <v>101</v>
       </c>
       <c r="Q39" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -4471,7 +4642,7 @@
         <v>101</v>
       </c>
       <c r="Q40" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -4525,7 +4696,7 @@
         <v>101</v>
       </c>
       <c r="Q41" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -6931,7 +7102,7 @@
         <v>101</v>
       </c>
       <c r="Q85" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="R85" s="7"/>
     </row>
@@ -9241,7 +9412,7 @@
         <v>101</v>
       </c>
       <c r="Q127" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="R127" s="7"/>
     </row>
@@ -9296,7 +9467,7 @@
         <v>101</v>
       </c>
       <c r="Q128" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="R128" s="7"/>
     </row>
@@ -25093,7 +25264,7 @@
         <v>505</v>
       </c>
       <c r="C416" s="7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D416" s="1" t="s">
         <v>514</v>
@@ -25107,7 +25278,7 @@
         <v>@SR00_001D@</v>
       </c>
       <c r="G416" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H416" s="8">
         <v>0</v>
@@ -25148,7 +25319,7 @@
         <v>505</v>
       </c>
       <c r="C417" s="2">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D417" s="1" t="s">
         <v>514</v>
@@ -25162,7 +25333,7 @@
         <v>@SR00_002D@</v>
       </c>
       <c r="G417" s="5">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H417" s="8">
         <v>0</v>
@@ -25191,7 +25362,7 @@
         <v>515</v>
       </c>
       <c r="Q417" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R417" s="7"/>
     </row>
@@ -25203,7 +25374,7 @@
         <v>505</v>
       </c>
       <c r="C418" s="7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D418" s="1" t="s">
         <v>513</v>
@@ -25217,7 +25388,7 @@
         <v>@SR00_003D@</v>
       </c>
       <c r="G418" s="8">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H418" s="8">
         <v>0</v>
@@ -25246,7 +25417,7 @@
         <v>515</v>
       </c>
       <c r="Q418" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="R418" s="7"/>
     </row>
@@ -25258,7 +25429,7 @@
         <v>505</v>
       </c>
       <c r="C419" s="2">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D419" s="1" t="s">
         <v>513</v>
@@ -25272,7 +25443,7 @@
         <v>@SR00_004D@</v>
       </c>
       <c r="G419" s="5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H419" s="8">
         <v>0</v>
@@ -25301,7 +25472,7 @@
         <v>515</v>
       </c>
       <c r="Q419" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="R419" s="7"/>
     </row>
@@ -25313,7 +25484,7 @@
         <v>505</v>
       </c>
       <c r="C420" s="7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D420" s="1" t="s">
         <v>513</v>
@@ -25327,7 +25498,7 @@
         <v>@SR00_005D@</v>
       </c>
       <c r="G420" s="8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H420" s="8">
         <v>0</v>
@@ -25356,7 +25527,7 @@
         <v>515</v>
       </c>
       <c r="Q420" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R420" s="7"/>
     </row>
@@ -25368,7 +25539,7 @@
         <v>505</v>
       </c>
       <c r="C421" s="2">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D421" s="1" t="s">
         <v>513</v>
@@ -25382,7 +25553,7 @@
         <v>@SR00_006D@</v>
       </c>
       <c r="G421" s="5">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="H421" s="8">
         <v>0</v>
@@ -25411,7 +25582,7 @@
         <v>515</v>
       </c>
       <c r="Q421" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R421" s="7"/>
     </row>
@@ -25423,7 +25594,7 @@
         <v>505</v>
       </c>
       <c r="C422" s="7">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="D422" s="1" t="s">
         <v>513</v>
@@ -25437,7 +25608,7 @@
         <v>@SR00_007D@</v>
       </c>
       <c r="G422" s="8">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="H422" s="8">
         <v>0</v>
@@ -25466,7 +25637,7 @@
         <v>515</v>
       </c>
       <c r="Q422" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R422" s="7"/>
     </row>
@@ -25478,7 +25649,7 @@
         <v>505</v>
       </c>
       <c r="C423" s="2">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="D423" s="1" t="s">
         <v>513</v>
@@ -25492,7 +25663,7 @@
         <v>@SR00_008D@</v>
       </c>
       <c r="G423" s="5">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="H423" s="8">
         <v>0</v>
@@ -25521,7 +25692,7 @@
         <v>515</v>
       </c>
       <c r="Q423" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R423" s="7"/>
     </row>
@@ -25533,7 +25704,7 @@
         <v>505</v>
       </c>
       <c r="C424" s="7">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="D424" s="1" t="s">
         <v>513</v>
@@ -25547,7 +25718,7 @@
         <v>@SR00_009D@</v>
       </c>
       <c r="G424" s="8">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H424" s="8">
         <v>0</v>
@@ -25576,7 +25747,7 @@
         <v>515</v>
       </c>
       <c r="Q424" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="R424" s="7"/>
     </row>
@@ -25588,7 +25759,7 @@
         <v>505</v>
       </c>
       <c r="C425" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D425" s="1" t="s">
         <v>513</v>
@@ -25602,7 +25773,7 @@
         <v>@SR00_010D@</v>
       </c>
       <c r="G425" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H425" s="8">
         <v>0</v>
@@ -25631,7 +25802,7 @@
         <v>515</v>
       </c>
       <c r="Q425" s="2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="R425" s="7"/>
     </row>
@@ -25643,7 +25814,7 @@
         <v>505</v>
       </c>
       <c r="C426" s="7">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="D426" s="1" t="s">
         <v>513</v>
@@ -25657,7 +25828,7 @@
         <v>@SR00_011D@</v>
       </c>
       <c r="G426" s="8">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="H426" s="8">
         <v>0</v>
@@ -25686,7 +25857,7 @@
         <v>515</v>
       </c>
       <c r="Q426" s="2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="R426" s="7"/>
     </row>
@@ -25698,7 +25869,7 @@
         <v>505</v>
       </c>
       <c r="C427" s="2">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="D427" s="1" t="s">
         <v>513</v>
@@ -25712,7 +25883,7 @@
         <v>@SR00_012D@</v>
       </c>
       <c r="G427" s="5">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="H427" s="8">
         <v>0</v>
@@ -25741,7 +25912,7 @@
         <v>515</v>
       </c>
       <c r="Q427" s="2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="R427" s="7"/>
     </row>
@@ -25753,7 +25924,7 @@
         <v>505</v>
       </c>
       <c r="C428" s="7">
-        <v>260</v>
+        <v>130</v>
       </c>
       <c r="D428" s="1" t="s">
         <v>513</v>
@@ -25767,7 +25938,7 @@
         <v>@SR00_013D@</v>
       </c>
       <c r="G428" s="8">
-        <v>260</v>
+        <v>130</v>
       </c>
       <c r="H428" s="8">
         <v>0</v>
@@ -25796,7 +25967,7 @@
         <v>515</v>
       </c>
       <c r="Q428" s="2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="R428" s="7"/>
     </row>
@@ -25808,7 +25979,7 @@
         <v>505</v>
       </c>
       <c r="C429" s="2">
-        <v>280</v>
+        <v>140</v>
       </c>
       <c r="D429" s="1" t="s">
         <v>513</v>
@@ -25822,7 +25993,7 @@
         <v>@SR00_014D@</v>
       </c>
       <c r="G429" s="5">
-        <v>280</v>
+        <v>140</v>
       </c>
       <c r="H429" s="8">
         <v>0</v>
@@ -25851,7 +26022,7 @@
         <v>515</v>
       </c>
       <c r="Q429" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R429" s="7"/>
     </row>
@@ -25863,7 +26034,7 @@
         <v>505</v>
       </c>
       <c r="C430" s="7">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D430" s="1" t="s">
         <v>513</v>
@@ -25877,7 +26048,7 @@
         <v>@SR00_015D@</v>
       </c>
       <c r="G430" s="8">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="H430" s="8">
         <v>0</v>
@@ -25906,7 +26077,7 @@
         <v>515</v>
       </c>
       <c r="Q430" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R430" s="7"/>
     </row>
@@ -25918,7 +26089,7 @@
         <v>505</v>
       </c>
       <c r="C431" s="2">
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="D431" s="1" t="s">
         <v>513</v>
@@ -25932,7 +26103,7 @@
         <v>@SR00_016D@</v>
       </c>
       <c r="G431" s="5">
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="H431" s="8">
         <v>0</v>
@@ -25961,7 +26132,7 @@
         <v>515</v>
       </c>
       <c r="Q431" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R431" s="7"/>
     </row>
@@ -25973,7 +26144,7 @@
         <v>505</v>
       </c>
       <c r="C432" s="7">
-        <v>340</v>
+        <v>170</v>
       </c>
       <c r="D432" s="1" t="s">
         <v>513</v>
@@ -25987,7 +26158,7 @@
         <v>@SR00_017D@</v>
       </c>
       <c r="G432" s="8">
-        <v>340</v>
+        <v>170</v>
       </c>
       <c r="H432" s="8">
         <v>0</v>
@@ -26016,7 +26187,7 @@
         <v>515</v>
       </c>
       <c r="Q432" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R432" s="7"/>
     </row>
@@ -26028,7 +26199,7 @@
         <v>505</v>
       </c>
       <c r="C433" s="2">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="D433" s="1" t="s">
         <v>513</v>
@@ -26042,7 +26213,7 @@
         <v>@SR00_018D@</v>
       </c>
       <c r="G433" s="5">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="H433" s="8">
         <v>0</v>
@@ -26071,7 +26242,7 @@
         <v>515</v>
       </c>
       <c r="Q433" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R433" s="7"/>
     </row>
@@ -26083,7 +26254,7 @@
         <v>505</v>
       </c>
       <c r="C434" s="7">
-        <v>380</v>
+        <v>190</v>
       </c>
       <c r="D434" s="1" t="s">
         <v>513</v>
@@ -26097,7 +26268,7 @@
         <v>@SR00_019D@</v>
       </c>
       <c r="G434" s="8">
-        <v>380</v>
+        <v>190</v>
       </c>
       <c r="H434" s="8">
         <v>0</v>
@@ -26126,7 +26297,7 @@
         <v>515</v>
       </c>
       <c r="Q434" s="2">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R434" s="7"/>
     </row>
@@ -26138,7 +26309,7 @@
         <v>505</v>
       </c>
       <c r="C435" s="2">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D435" s="1" t="s">
         <v>513</v>
@@ -26152,7 +26323,7 @@
         <v>@SR00_020D@</v>
       </c>
       <c r="G435" s="5">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="H435" s="8">
         <v>0</v>
@@ -26181,7 +26352,7 @@
         <v>515</v>
       </c>
       <c r="Q435" s="2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="R435" s="7"/>
     </row>
@@ -26193,7 +26364,7 @@
         <v>505</v>
       </c>
       <c r="C436" s="7">
-        <v>420</v>
+        <v>210</v>
       </c>
       <c r="D436" s="1" t="s">
         <v>513</v>
@@ -26207,7 +26378,7 @@
         <v>@SR00_021D@</v>
       </c>
       <c r="G436" s="8">
-        <v>420</v>
+        <v>210</v>
       </c>
       <c r="H436" s="8">
         <v>0</v>
@@ -26236,7 +26407,7 @@
         <v>515</v>
       </c>
       <c r="Q436" s="2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="R436" s="7"/>
     </row>
@@ -26248,7 +26419,7 @@
         <v>505</v>
       </c>
       <c r="C437" s="2">
-        <v>440</v>
+        <v>220</v>
       </c>
       <c r="D437" s="1" t="s">
         <v>513</v>
@@ -26262,7 +26433,7 @@
         <v>@SR00_022D@</v>
       </c>
       <c r="G437" s="5">
-        <v>440</v>
+        <v>220</v>
       </c>
       <c r="H437" s="8">
         <v>0</v>
@@ -26291,7 +26462,7 @@
         <v>515</v>
       </c>
       <c r="Q437" s="2">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="R437" s="7"/>
     </row>
@@ -26303,7 +26474,7 @@
         <v>505</v>
       </c>
       <c r="C438" s="7">
-        <v>460</v>
+        <v>230</v>
       </c>
       <c r="D438" s="1" t="s">
         <v>513</v>
@@ -26317,7 +26488,7 @@
         <v>@SR00_023D@</v>
       </c>
       <c r="G438" s="8">
-        <v>460</v>
+        <v>230</v>
       </c>
       <c r="H438" s="8">
         <v>0</v>
@@ -26346,7 +26517,7 @@
         <v>515</v>
       </c>
       <c r="Q438" s="2">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="R438" s="7"/>
     </row>
@@ -26358,7 +26529,7 @@
         <v>505</v>
       </c>
       <c r="C439" s="2">
-        <v>480</v>
+        <v>240</v>
       </c>
       <c r="D439" s="1" t="s">
         <v>513</v>
@@ -26372,7 +26543,7 @@
         <v>@SR00_024D@</v>
       </c>
       <c r="G439" s="5">
-        <v>480</v>
+        <v>240</v>
       </c>
       <c r="H439" s="8">
         <v>0</v>
@@ -26401,7 +26572,7 @@
         <v>515</v>
       </c>
       <c r="Q439" s="2">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="R439" s="7"/>
     </row>
@@ -26413,7 +26584,7 @@
         <v>505</v>
       </c>
       <c r="C440" s="7">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D440" s="1" t="s">
         <v>513</v>
@@ -26427,7 +26598,7 @@
         <v>@SR00_025D@</v>
       </c>
       <c r="G440" s="8">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="H440" s="8">
         <v>0</v>
@@ -26456,7 +26627,7 @@
         <v>515</v>
       </c>
       <c r="Q440" s="2">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="R440" s="7"/>
     </row>
@@ -26468,7 +26639,7 @@
         <v>505</v>
       </c>
       <c r="C441" s="2">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="D441" s="1" t="s">
         <v>513</v>
@@ -26482,7 +26653,7 @@
         <v>@SR00_026D@</v>
       </c>
       <c r="G441" s="5">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="H441" s="8">
         <v>0</v>
@@ -26511,7 +26682,7 @@
         <v>515</v>
       </c>
       <c r="Q441" s="2">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="R441" s="7"/>
     </row>
@@ -26523,7 +26694,7 @@
         <v>505</v>
       </c>
       <c r="C442" s="7">
-        <v>540</v>
+        <v>270</v>
       </c>
       <c r="D442" s="1" t="s">
         <v>513</v>
@@ -26537,7 +26708,7 @@
         <v>@SR00_027D@</v>
       </c>
       <c r="G442" s="8">
-        <v>540</v>
+        <v>270</v>
       </c>
       <c r="H442" s="8">
         <v>0</v>
@@ -26566,7 +26737,7 @@
         <v>515</v>
       </c>
       <c r="Q442" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R442" s="7"/>
     </row>
@@ -26578,7 +26749,7 @@
         <v>505</v>
       </c>
       <c r="C443" s="2">
-        <v>560</v>
+        <v>280</v>
       </c>
       <c r="D443" s="1" t="s">
         <v>513</v>
@@ -26592,7 +26763,7 @@
         <v>@SR00_028D@</v>
       </c>
       <c r="G443" s="5">
-        <v>560</v>
+        <v>280</v>
       </c>
       <c r="H443" s="8">
         <v>0</v>
@@ -26621,7 +26792,7 @@
         <v>515</v>
       </c>
       <c r="Q443" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R443" s="7"/>
     </row>
@@ -26633,7 +26804,7 @@
         <v>505</v>
       </c>
       <c r="C444" s="7">
-        <v>580</v>
+        <v>290</v>
       </c>
       <c r="D444" s="1" t="s">
         <v>513</v>
@@ -26647,7 +26818,7 @@
         <v>@SR00_029D@</v>
       </c>
       <c r="G444" s="8">
-        <v>580</v>
+        <v>290</v>
       </c>
       <c r="H444" s="8">
         <v>0</v>
@@ -26676,7 +26847,7 @@
         <v>515</v>
       </c>
       <c r="Q444" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R444" s="7"/>
     </row>
@@ -26688,7 +26859,7 @@
         <v>505</v>
       </c>
       <c r="C445" s="2">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="D445" s="1" t="s">
         <v>513</v>
@@ -26702,7 +26873,7 @@
         <v>@SR00_030D@</v>
       </c>
       <c r="G445" s="5">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H445" s="8">
         <v>0</v>
@@ -26731,7 +26902,7 @@
         <v>515</v>
       </c>
       <c r="Q445" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R445" s="7"/>
     </row>
@@ -26743,7 +26914,7 @@
         <v>505</v>
       </c>
       <c r="C446" s="7">
-        <v>620</v>
+        <v>310</v>
       </c>
       <c r="D446" s="1" t="s">
         <v>513</v>
@@ -26757,7 +26928,7 @@
         <v>@SR00_031D@</v>
       </c>
       <c r="G446" s="8">
-        <v>620</v>
+        <v>310</v>
       </c>
       <c r="H446" s="8">
         <v>0</v>
@@ -26786,7 +26957,7 @@
         <v>515</v>
       </c>
       <c r="Q446" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R446" s="7"/>
     </row>
@@ -26798,7 +26969,7 @@
         <v>505</v>
       </c>
       <c r="C447" s="2">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="D447" s="1" t="s">
         <v>513</v>
@@ -26812,7 +26983,7 @@
         <v>@SR00_032D@</v>
       </c>
       <c r="G447" s="5">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="H447" s="8">
         <v>0</v>
@@ -26841,7 +27012,7 @@
         <v>515</v>
       </c>
       <c r="Q447" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R447" s="7"/>
     </row>
@@ -26853,7 +27024,7 @@
         <v>505</v>
       </c>
       <c r="C448" s="7">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="D448" s="1" t="s">
         <v>513</v>
@@ -26867,7 +27038,7 @@
         <v>@SR00_033D@</v>
       </c>
       <c r="G448" s="8">
-        <v>660</v>
+        <v>330</v>
       </c>
       <c r="H448" s="8">
         <v>0</v>
@@ -26896,7 +27067,7 @@
         <v>515</v>
       </c>
       <c r="Q448" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R448" s="7"/>
     </row>
@@ -26908,7 +27079,7 @@
         <v>505</v>
       </c>
       <c r="C449" s="2">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="D449" s="1" t="s">
         <v>513</v>
@@ -26922,7 +27093,7 @@
         <v>@SR00_034D@</v>
       </c>
       <c r="G449" s="5">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="H449" s="8">
         <v>0</v>
@@ -26951,7 +27122,7 @@
         <v>515</v>
       </c>
       <c r="Q449" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R449" s="7"/>
     </row>
@@ -26963,7 +27134,7 @@
         <v>505</v>
       </c>
       <c r="C450" s="7">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="D450" s="1" t="s">
         <v>513</v>
@@ -26977,7 +27148,7 @@
         <v>@SR00_035D@</v>
       </c>
       <c r="G450" s="8">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="H450" s="8">
         <v>0</v>
@@ -27006,7 +27177,7 @@
         <v>515</v>
       </c>
       <c r="Q450" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R450" s="7"/>
     </row>
@@ -27018,7 +27189,7 @@
         <v>505</v>
       </c>
       <c r="C451" s="2">
-        <v>720</v>
+        <v>360</v>
       </c>
       <c r="D451" s="1" t="s">
         <v>513</v>
@@ -27032,7 +27203,7 @@
         <v>@SR00_036D@</v>
       </c>
       <c r="G451" s="5">
-        <v>720</v>
+        <v>360</v>
       </c>
       <c r="H451" s="8">
         <v>0</v>
@@ -27061,7 +27232,7 @@
         <v>515</v>
       </c>
       <c r="Q451" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R451" s="7"/>
     </row>
@@ -27073,7 +27244,7 @@
         <v>505</v>
       </c>
       <c r="C452" s="7">
-        <v>740</v>
+        <v>370</v>
       </c>
       <c r="D452" s="1" t="s">
         <v>513</v>
@@ -27087,7 +27258,7 @@
         <v>@SR00_037D@</v>
       </c>
       <c r="G452" s="8">
-        <v>740</v>
+        <v>370</v>
       </c>
       <c r="H452" s="8">
         <v>0</v>
@@ -27116,7 +27287,7 @@
         <v>515</v>
       </c>
       <c r="Q452" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="R452" s="7"/>
     </row>
@@ -27128,7 +27299,7 @@
         <v>505</v>
       </c>
       <c r="C453" s="2">
-        <v>760</v>
+        <v>380</v>
       </c>
       <c r="D453" s="1" t="s">
         <v>513</v>
@@ -27142,7 +27313,7 @@
         <v>@SR00_038D@</v>
       </c>
       <c r="G453" s="5">
-        <v>760</v>
+        <v>380</v>
       </c>
       <c r="H453" s="8">
         <v>0</v>
@@ -27171,7 +27342,7 @@
         <v>515</v>
       </c>
       <c r="Q453" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="R453" s="7"/>
     </row>
@@ -27183,7 +27354,7 @@
         <v>505</v>
       </c>
       <c r="C454" s="7">
-        <v>780</v>
+        <v>390</v>
       </c>
       <c r="D454" s="1" t="s">
         <v>513</v>
@@ -27197,7 +27368,7 @@
         <v>@SR00_039D@</v>
       </c>
       <c r="G454" s="8">
-        <v>780</v>
+        <v>390</v>
       </c>
       <c r="H454" s="8">
         <v>0</v>
@@ -27226,7 +27397,7 @@
         <v>515</v>
       </c>
       <c r="Q454" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="R454" s="7"/>
     </row>
@@ -27238,7 +27409,7 @@
         <v>505</v>
       </c>
       <c r="C455" s="2">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="D455" s="1" t="s">
         <v>513</v>
@@ -27252,7 +27423,7 @@
         <v>@SR00_040D@</v>
       </c>
       <c r="G455" s="5">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="H455" s="8">
         <v>0</v>
@@ -27281,7 +27452,7 @@
         <v>515</v>
       </c>
       <c r="Q455" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R455" s="7"/>
     </row>
@@ -27293,7 +27464,7 @@
         <v>505</v>
       </c>
       <c r="C456" s="7">
-        <v>820</v>
+        <v>410</v>
       </c>
       <c r="D456" s="1" t="s">
         <v>513</v>
@@ -27307,7 +27478,7 @@
         <v>@SR00_041D@</v>
       </c>
       <c r="G456" s="8">
-        <v>820</v>
+        <v>410</v>
       </c>
       <c r="H456" s="8">
         <v>0</v>
@@ -27336,7 +27507,7 @@
         <v>515</v>
       </c>
       <c r="Q456" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R456" s="7"/>
     </row>
@@ -27348,7 +27519,7 @@
         <v>505</v>
       </c>
       <c r="C457" s="2">
-        <v>840</v>
+        <v>420</v>
       </c>
       <c r="D457" s="1" t="s">
         <v>513</v>
@@ -27362,7 +27533,7 @@
         <v>@SR00_042D@</v>
       </c>
       <c r="G457" s="5">
-        <v>840</v>
+        <v>420</v>
       </c>
       <c r="H457" s="8">
         <v>0</v>
@@ -27391,7 +27562,7 @@
         <v>515</v>
       </c>
       <c r="Q457" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R457" s="7"/>
     </row>
@@ -27403,7 +27574,7 @@
         <v>505</v>
       </c>
       <c r="C458" s="7">
-        <v>860</v>
+        <v>430</v>
       </c>
       <c r="D458" s="1" t="s">
         <v>513</v>
@@ -27417,7 +27588,7 @@
         <v>@SR00_043D@</v>
       </c>
       <c r="G458" s="8">
-        <v>860</v>
+        <v>430</v>
       </c>
       <c r="H458" s="8">
         <v>0</v>
@@ -27446,7 +27617,7 @@
         <v>515</v>
       </c>
       <c r="Q458" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R458" s="7"/>
     </row>
@@ -27458,7 +27629,7 @@
         <v>505</v>
       </c>
       <c r="C459" s="2">
-        <v>880</v>
+        <v>440</v>
       </c>
       <c r="D459" s="1" t="s">
         <v>513</v>
@@ -27472,7 +27643,7 @@
         <v>@SR00_044D@</v>
       </c>
       <c r="G459" s="5">
-        <v>880</v>
+        <v>440</v>
       </c>
       <c r="H459" s="8">
         <v>0</v>
@@ -27501,7 +27672,7 @@
         <v>515</v>
       </c>
       <c r="Q459" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R459" s="7"/>
     </row>
@@ -27513,7 +27684,7 @@
         <v>505</v>
       </c>
       <c r="C460" s="7">
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="D460" s="1" t="s">
         <v>513</v>
@@ -27527,7 +27698,7 @@
         <v>@SR00_045D@</v>
       </c>
       <c r="G460" s="8">
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="H460" s="8">
         <v>0</v>
@@ -27556,9 +27727,2484 @@
         <v>515</v>
       </c>
       <c r="Q460" s="2">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="R460" s="7"/>
+    </row>
+    <row r="461" spans="1:18">
+      <c r="A461" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="B461" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C461" s="2">
+        <v>460</v>
+      </c>
+      <c r="D461" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E461" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_046N@</v>
+      </c>
+      <c r="F461" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_046D@</v>
+      </c>
+      <c r="G461" s="5">
+        <v>460</v>
+      </c>
+      <c r="H461" s="8">
+        <v>0</v>
+      </c>
+      <c r="I461" s="8">
+        <v>50</v>
+      </c>
+      <c r="J461" s="7">
+        <v>70</v>
+      </c>
+      <c r="K461" s="7">
+        <v>30</v>
+      </c>
+      <c r="L461" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_046</v>
+      </c>
+      <c r="N461" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_046</v>
+      </c>
+      <c r="O461" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P461" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q461" s="2">
+        <v>4</v>
+      </c>
+      <c r="R461" s="7"/>
+    </row>
+    <row r="462" spans="1:18">
+      <c r="A462" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="B462" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C462" s="7">
+        <v>470</v>
+      </c>
+      <c r="D462" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E462" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_047N@</v>
+      </c>
+      <c r="F462" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_047D@</v>
+      </c>
+      <c r="G462" s="8">
+        <v>470</v>
+      </c>
+      <c r="H462" s="8">
+        <v>0</v>
+      </c>
+      <c r="I462" s="8">
+        <v>50</v>
+      </c>
+      <c r="J462" s="7">
+        <v>70</v>
+      </c>
+      <c r="K462" s="7">
+        <v>30</v>
+      </c>
+      <c r="L462" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_047</v>
+      </c>
+      <c r="N462" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_047</v>
+      </c>
+      <c r="O462" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P462" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q462" s="2">
+        <v>4</v>
+      </c>
+      <c r="R462" s="7"/>
+    </row>
+    <row r="463" spans="1:18">
+      <c r="A463" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="B463" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C463" s="2">
+        <v>480</v>
+      </c>
+      <c r="D463" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E463" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_048N@</v>
+      </c>
+      <c r="F463" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_048D@</v>
+      </c>
+      <c r="G463" s="5">
+        <v>480</v>
+      </c>
+      <c r="H463" s="8">
+        <v>0</v>
+      </c>
+      <c r="I463" s="8">
+        <v>50</v>
+      </c>
+      <c r="J463" s="7">
+        <v>70</v>
+      </c>
+      <c r="K463" s="7">
+        <v>30</v>
+      </c>
+      <c r="L463" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_048</v>
+      </c>
+      <c r="N463" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_048</v>
+      </c>
+      <c r="O463" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P463" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q463" s="2">
+        <v>4</v>
+      </c>
+      <c r="R463" s="7"/>
+    </row>
+    <row r="464" spans="1:18">
+      <c r="A464" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="B464" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C464" s="7">
+        <v>490</v>
+      </c>
+      <c r="D464" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E464" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_049N@</v>
+      </c>
+      <c r="F464" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_049D@</v>
+      </c>
+      <c r="G464" s="8">
+        <v>490</v>
+      </c>
+      <c r="H464" s="8">
+        <v>0</v>
+      </c>
+      <c r="I464" s="8">
+        <v>50</v>
+      </c>
+      <c r="J464" s="7">
+        <v>70</v>
+      </c>
+      <c r="K464" s="7">
+        <v>30</v>
+      </c>
+      <c r="L464" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_049</v>
+      </c>
+      <c r="N464" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_049</v>
+      </c>
+      <c r="O464" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P464" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q464" s="2">
+        <v>4</v>
+      </c>
+      <c r="R464" s="7"/>
+    </row>
+    <row r="465" spans="1:18">
+      <c r="A465" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="B465" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C465" s="2">
+        <v>500</v>
+      </c>
+      <c r="D465" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E465" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_050N@</v>
+      </c>
+      <c r="F465" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_050D@</v>
+      </c>
+      <c r="G465" s="5">
+        <v>500</v>
+      </c>
+      <c r="H465" s="8">
+        <v>0</v>
+      </c>
+      <c r="I465" s="8">
+        <v>50</v>
+      </c>
+      <c r="J465" s="7">
+        <v>70</v>
+      </c>
+      <c r="K465" s="7">
+        <v>30</v>
+      </c>
+      <c r="L465" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_050</v>
+      </c>
+      <c r="N465" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_050</v>
+      </c>
+      <c r="O465" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P465" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q465" s="2">
+        <v>4</v>
+      </c>
+      <c r="R465" s="7"/>
+    </row>
+    <row r="466" spans="1:18">
+      <c r="A466" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B466" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C466" s="7">
+        <v>510</v>
+      </c>
+      <c r="D466" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E466" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_051N@</v>
+      </c>
+      <c r="F466" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_051D@</v>
+      </c>
+      <c r="G466" s="8">
+        <v>510</v>
+      </c>
+      <c r="H466" s="8">
+        <v>0</v>
+      </c>
+      <c r="I466" s="8">
+        <v>50</v>
+      </c>
+      <c r="J466" s="7">
+        <v>70</v>
+      </c>
+      <c r="K466" s="7">
+        <v>30</v>
+      </c>
+      <c r="L466" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_051</v>
+      </c>
+      <c r="N466" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_051</v>
+      </c>
+      <c r="O466" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P466" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q466" s="2">
+        <v>3</v>
+      </c>
+      <c r="R466" s="7"/>
+    </row>
+    <row r="467" spans="1:18">
+      <c r="A467" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="B467" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C467" s="2">
+        <v>520</v>
+      </c>
+      <c r="D467" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E467" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_052N@</v>
+      </c>
+      <c r="F467" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_052D@</v>
+      </c>
+      <c r="G467" s="5">
+        <v>520</v>
+      </c>
+      <c r="H467" s="8">
+        <v>0</v>
+      </c>
+      <c r="I467" s="8">
+        <v>50</v>
+      </c>
+      <c r="J467" s="7">
+        <v>70</v>
+      </c>
+      <c r="K467" s="7">
+        <v>30</v>
+      </c>
+      <c r="L467" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_052</v>
+      </c>
+      <c r="N467" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_052</v>
+      </c>
+      <c r="O467" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P467" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q467" s="2">
+        <v>3</v>
+      </c>
+      <c r="R467" s="7"/>
+    </row>
+    <row r="468" spans="1:18">
+      <c r="A468" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="B468" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C468" s="7">
+        <v>530</v>
+      </c>
+      <c r="D468" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E468" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_053N@</v>
+      </c>
+      <c r="F468" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_053D@</v>
+      </c>
+      <c r="G468" s="8">
+        <v>530</v>
+      </c>
+      <c r="H468" s="8">
+        <v>0</v>
+      </c>
+      <c r="I468" s="8">
+        <v>50</v>
+      </c>
+      <c r="J468" s="7">
+        <v>70</v>
+      </c>
+      <c r="K468" s="7">
+        <v>30</v>
+      </c>
+      <c r="L468" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_053</v>
+      </c>
+      <c r="N468" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_053</v>
+      </c>
+      <c r="O468" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P468" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q468" s="2">
+        <v>3</v>
+      </c>
+      <c r="R468" s="7"/>
+    </row>
+    <row r="469" spans="1:18">
+      <c r="A469" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="B469" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C469" s="2">
+        <v>540</v>
+      </c>
+      <c r="D469" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E469" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_054N@</v>
+      </c>
+      <c r="F469" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_054D@</v>
+      </c>
+      <c r="G469" s="5">
+        <v>540</v>
+      </c>
+      <c r="H469" s="8">
+        <v>0</v>
+      </c>
+      <c r="I469" s="8">
+        <v>50</v>
+      </c>
+      <c r="J469" s="7">
+        <v>70</v>
+      </c>
+      <c r="K469" s="7">
+        <v>30</v>
+      </c>
+      <c r="L469" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_054</v>
+      </c>
+      <c r="N469" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_054</v>
+      </c>
+      <c r="O469" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P469" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q469" s="2">
+        <v>4</v>
+      </c>
+      <c r="R469" s="7"/>
+    </row>
+    <row r="470" spans="1:18">
+      <c r="A470" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B470" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C470" s="7">
+        <v>550</v>
+      </c>
+      <c r="D470" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E470" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_055N@</v>
+      </c>
+      <c r="F470" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_055D@</v>
+      </c>
+      <c r="G470" s="8">
+        <v>550</v>
+      </c>
+      <c r="H470" s="8">
+        <v>0</v>
+      </c>
+      <c r="I470" s="8">
+        <v>50</v>
+      </c>
+      <c r="J470" s="7">
+        <v>70</v>
+      </c>
+      <c r="K470" s="7">
+        <v>30</v>
+      </c>
+      <c r="L470" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_055</v>
+      </c>
+      <c r="N470" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_055</v>
+      </c>
+      <c r="O470" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P470" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q470" s="2">
+        <v>4</v>
+      </c>
+      <c r="R470" s="7"/>
+    </row>
+    <row r="471" spans="1:18">
+      <c r="A471" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="B471" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C471" s="2">
+        <v>560</v>
+      </c>
+      <c r="D471" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E471" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_056N@</v>
+      </c>
+      <c r="F471" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_056D@</v>
+      </c>
+      <c r="G471" s="5">
+        <v>560</v>
+      </c>
+      <c r="H471" s="8">
+        <v>0</v>
+      </c>
+      <c r="I471" s="8">
+        <v>50</v>
+      </c>
+      <c r="J471" s="7">
+        <v>70</v>
+      </c>
+      <c r="K471" s="7">
+        <v>30</v>
+      </c>
+      <c r="L471" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_056</v>
+      </c>
+      <c r="N471" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_056</v>
+      </c>
+      <c r="O471" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P471" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q471" s="2">
+        <v>4</v>
+      </c>
+      <c r="R471" s="7"/>
+    </row>
+    <row r="472" spans="1:18">
+      <c r="A472" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="B472" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C472" s="7">
+        <v>570</v>
+      </c>
+      <c r="D472" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E472" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_057N@</v>
+      </c>
+      <c r="F472" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_057D@</v>
+      </c>
+      <c r="G472" s="8">
+        <v>570</v>
+      </c>
+      <c r="H472" s="8">
+        <v>0</v>
+      </c>
+      <c r="I472" s="8">
+        <v>50</v>
+      </c>
+      <c r="J472" s="7">
+        <v>70</v>
+      </c>
+      <c r="K472" s="7">
+        <v>30</v>
+      </c>
+      <c r="L472" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_057</v>
+      </c>
+      <c r="N472" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_057</v>
+      </c>
+      <c r="O472" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P472" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q472" s="2">
+        <v>4</v>
+      </c>
+      <c r="R472" s="7"/>
+    </row>
+    <row r="473" spans="1:18">
+      <c r="A473" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="B473" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C473" s="2">
+        <v>580</v>
+      </c>
+      <c r="D473" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E473" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_058N@</v>
+      </c>
+      <c r="F473" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_058D@</v>
+      </c>
+      <c r="G473" s="5">
+        <v>580</v>
+      </c>
+      <c r="H473" s="8">
+        <v>0</v>
+      </c>
+      <c r="I473" s="8">
+        <v>50</v>
+      </c>
+      <c r="J473" s="7">
+        <v>70</v>
+      </c>
+      <c r="K473" s="7">
+        <v>30</v>
+      </c>
+      <c r="L473" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_058</v>
+      </c>
+      <c r="N473" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_058</v>
+      </c>
+      <c r="O473" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P473" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q473" s="2">
+        <v>4</v>
+      </c>
+      <c r="R473" s="7"/>
+    </row>
+    <row r="474" spans="1:18">
+      <c r="A474" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="B474" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C474" s="7">
+        <v>590</v>
+      </c>
+      <c r="D474" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E474" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_059N@</v>
+      </c>
+      <c r="F474" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_059D@</v>
+      </c>
+      <c r="G474" s="8">
+        <v>590</v>
+      </c>
+      <c r="H474" s="8">
+        <v>0</v>
+      </c>
+      <c r="I474" s="8">
+        <v>50</v>
+      </c>
+      <c r="J474" s="7">
+        <v>70</v>
+      </c>
+      <c r="K474" s="7">
+        <v>30</v>
+      </c>
+      <c r="L474" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_059</v>
+      </c>
+      <c r="N474" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_059</v>
+      </c>
+      <c r="O474" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P474" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q474" s="2">
+        <v>4</v>
+      </c>
+      <c r="R474" s="7"/>
+    </row>
+    <row r="475" spans="1:18">
+      <c r="A475" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B475" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C475" s="2">
+        <v>600</v>
+      </c>
+      <c r="D475" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E475" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_060N@</v>
+      </c>
+      <c r="F475" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_060D@</v>
+      </c>
+      <c r="G475" s="5">
+        <v>600</v>
+      </c>
+      <c r="H475" s="8">
+        <v>0</v>
+      </c>
+      <c r="I475" s="8">
+        <v>50</v>
+      </c>
+      <c r="J475" s="7">
+        <v>70</v>
+      </c>
+      <c r="K475" s="7">
+        <v>30</v>
+      </c>
+      <c r="L475" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_060</v>
+      </c>
+      <c r="N475" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_060</v>
+      </c>
+      <c r="O475" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P475" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q475" s="2">
+        <v>4</v>
+      </c>
+      <c r="R475" s="7"/>
+    </row>
+    <row r="476" spans="1:18">
+      <c r="A476" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B476" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C476" s="7">
+        <v>610</v>
+      </c>
+      <c r="D476" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E476" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_061N@</v>
+      </c>
+      <c r="F476" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_061D@</v>
+      </c>
+      <c r="G476" s="8">
+        <v>610</v>
+      </c>
+      <c r="H476" s="8">
+        <v>0</v>
+      </c>
+      <c r="I476" s="8">
+        <v>50</v>
+      </c>
+      <c r="J476" s="7">
+        <v>70</v>
+      </c>
+      <c r="K476" s="7">
+        <v>30</v>
+      </c>
+      <c r="L476" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_061</v>
+      </c>
+      <c r="N476" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_061</v>
+      </c>
+      <c r="O476" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P476" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q476" s="2">
+        <v>4</v>
+      </c>
+      <c r="R476" s="7"/>
+    </row>
+    <row r="477" spans="1:18">
+      <c r="A477" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="B477" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C477" s="2">
+        <v>620</v>
+      </c>
+      <c r="D477" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E477" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_062N@</v>
+      </c>
+      <c r="F477" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_062D@</v>
+      </c>
+      <c r="G477" s="5">
+        <v>620</v>
+      </c>
+      <c r="H477" s="8">
+        <v>0</v>
+      </c>
+      <c r="I477" s="8">
+        <v>50</v>
+      </c>
+      <c r="J477" s="7">
+        <v>70</v>
+      </c>
+      <c r="K477" s="7">
+        <v>30</v>
+      </c>
+      <c r="L477" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_062</v>
+      </c>
+      <c r="N477" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_062</v>
+      </c>
+      <c r="O477" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P477" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q477" s="2">
+        <v>4</v>
+      </c>
+      <c r="R477" s="7"/>
+    </row>
+    <row r="478" spans="1:18">
+      <c r="A478" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="B478" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C478" s="7">
+        <v>630</v>
+      </c>
+      <c r="D478" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E478" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_063N@</v>
+      </c>
+      <c r="F478" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_063D@</v>
+      </c>
+      <c r="G478" s="8">
+        <v>630</v>
+      </c>
+      <c r="H478" s="8">
+        <v>0</v>
+      </c>
+      <c r="I478" s="8">
+        <v>50</v>
+      </c>
+      <c r="J478" s="7">
+        <v>70</v>
+      </c>
+      <c r="K478" s="7">
+        <v>30</v>
+      </c>
+      <c r="L478" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_063</v>
+      </c>
+      <c r="N478" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_063</v>
+      </c>
+      <c r="O478" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P478" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q478" s="2">
+        <v>3</v>
+      </c>
+      <c r="R478" s="7"/>
+    </row>
+    <row r="479" spans="1:18">
+      <c r="A479" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B479" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C479" s="2">
+        <v>640</v>
+      </c>
+      <c r="D479" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E479" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_064N@</v>
+      </c>
+      <c r="F479" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_064D@</v>
+      </c>
+      <c r="G479" s="5">
+        <v>640</v>
+      </c>
+      <c r="H479" s="8">
+        <v>0</v>
+      </c>
+      <c r="I479" s="8">
+        <v>50</v>
+      </c>
+      <c r="J479" s="7">
+        <v>70</v>
+      </c>
+      <c r="K479" s="7">
+        <v>30</v>
+      </c>
+      <c r="L479" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_064</v>
+      </c>
+      <c r="N479" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_064</v>
+      </c>
+      <c r="O479" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P479" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q479" s="2">
+        <v>3</v>
+      </c>
+      <c r="R479" s="7"/>
+    </row>
+    <row r="480" spans="1:18">
+      <c r="A480" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="B480" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C480" s="7">
+        <v>650</v>
+      </c>
+      <c r="D480" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E480" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_065N@</v>
+      </c>
+      <c r="F480" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_065D@</v>
+      </c>
+      <c r="G480" s="8">
+        <v>650</v>
+      </c>
+      <c r="H480" s="8">
+        <v>0</v>
+      </c>
+      <c r="I480" s="8">
+        <v>50</v>
+      </c>
+      <c r="J480" s="7">
+        <v>70</v>
+      </c>
+      <c r="K480" s="7">
+        <v>30</v>
+      </c>
+      <c r="L480" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_065</v>
+      </c>
+      <c r="N480" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_065</v>
+      </c>
+      <c r="O480" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P480" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q480" s="2">
+        <v>3</v>
+      </c>
+      <c r="R480" s="7"/>
+    </row>
+    <row r="481" spans="1:18">
+      <c r="A481" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="B481" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C481" s="2">
+        <v>660</v>
+      </c>
+      <c r="D481" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E481" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_066N@</v>
+      </c>
+      <c r="F481" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_066D@</v>
+      </c>
+      <c r="G481" s="5">
+        <v>660</v>
+      </c>
+      <c r="H481" s="8">
+        <v>0</v>
+      </c>
+      <c r="I481" s="8">
+        <v>50</v>
+      </c>
+      <c r="J481" s="7">
+        <v>70</v>
+      </c>
+      <c r="K481" s="7">
+        <v>30</v>
+      </c>
+      <c r="L481" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_066</v>
+      </c>
+      <c r="N481" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_066</v>
+      </c>
+      <c r="O481" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P481" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q481" s="2">
+        <v>4</v>
+      </c>
+      <c r="R481" s="7"/>
+    </row>
+    <row r="482" spans="1:18">
+      <c r="A482" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="B482" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C482" s="7">
+        <v>670</v>
+      </c>
+      <c r="D482" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E482" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_067N@</v>
+      </c>
+      <c r="F482" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_067D@</v>
+      </c>
+      <c r="G482" s="8">
+        <v>670</v>
+      </c>
+      <c r="H482" s="8">
+        <v>0</v>
+      </c>
+      <c r="I482" s="8">
+        <v>50</v>
+      </c>
+      <c r="J482" s="7">
+        <v>70</v>
+      </c>
+      <c r="K482" s="7">
+        <v>30</v>
+      </c>
+      <c r="L482" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_067</v>
+      </c>
+      <c r="N482" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_067</v>
+      </c>
+      <c r="O482" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P482" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q482" s="2">
+        <v>4</v>
+      </c>
+      <c r="R482" s="7"/>
+    </row>
+    <row r="483" spans="1:18">
+      <c r="A483" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="B483" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C483" s="2">
+        <v>680</v>
+      </c>
+      <c r="D483" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E483" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_068N@</v>
+      </c>
+      <c r="F483" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_068D@</v>
+      </c>
+      <c r="G483" s="5">
+        <v>680</v>
+      </c>
+      <c r="H483" s="8">
+        <v>0</v>
+      </c>
+      <c r="I483" s="8">
+        <v>50</v>
+      </c>
+      <c r="J483" s="7">
+        <v>70</v>
+      </c>
+      <c r="K483" s="7">
+        <v>30</v>
+      </c>
+      <c r="L483" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_068</v>
+      </c>
+      <c r="N483" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_068</v>
+      </c>
+      <c r="O483" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P483" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q483" s="2">
+        <v>4</v>
+      </c>
+      <c r="R483" s="7"/>
+    </row>
+    <row r="484" spans="1:18">
+      <c r="A484" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="B484" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C484" s="7">
+        <v>690</v>
+      </c>
+      <c r="D484" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E484" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_069N@</v>
+      </c>
+      <c r="F484" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_069D@</v>
+      </c>
+      <c r="G484" s="8">
+        <v>690</v>
+      </c>
+      <c r="H484" s="8">
+        <v>0</v>
+      </c>
+      <c r="I484" s="8">
+        <v>50</v>
+      </c>
+      <c r="J484" s="7">
+        <v>70</v>
+      </c>
+      <c r="K484" s="7">
+        <v>30</v>
+      </c>
+      <c r="L484" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_069</v>
+      </c>
+      <c r="N484" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_069</v>
+      </c>
+      <c r="O484" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P484" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q484" s="2">
+        <v>4</v>
+      </c>
+      <c r="R484" s="7"/>
+    </row>
+    <row r="485" spans="1:18">
+      <c r="A485" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="B485" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C485" s="2">
+        <v>700</v>
+      </c>
+      <c r="D485" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E485" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_070N@</v>
+      </c>
+      <c r="F485" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_070D@</v>
+      </c>
+      <c r="G485" s="5">
+        <v>700</v>
+      </c>
+      <c r="H485" s="8">
+        <v>0</v>
+      </c>
+      <c r="I485" s="8">
+        <v>50</v>
+      </c>
+      <c r="J485" s="7">
+        <v>70</v>
+      </c>
+      <c r="K485" s="7">
+        <v>30</v>
+      </c>
+      <c r="L485" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_070</v>
+      </c>
+      <c r="N485" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_070</v>
+      </c>
+      <c r="O485" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P485" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q485" s="2">
+        <v>4</v>
+      </c>
+      <c r="R485" s="7"/>
+    </row>
+    <row r="486" spans="1:18">
+      <c r="A486" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="B486" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C486" s="7">
+        <v>710</v>
+      </c>
+      <c r="D486" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E486" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_071N@</v>
+      </c>
+      <c r="F486" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_071D@</v>
+      </c>
+      <c r="G486" s="8">
+        <v>710</v>
+      </c>
+      <c r="H486" s="8">
+        <v>0</v>
+      </c>
+      <c r="I486" s="8">
+        <v>50</v>
+      </c>
+      <c r="J486" s="7">
+        <v>70</v>
+      </c>
+      <c r="K486" s="7">
+        <v>30</v>
+      </c>
+      <c r="L486" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_071</v>
+      </c>
+      <c r="N486" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_071</v>
+      </c>
+      <c r="O486" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P486" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q486" s="2">
+        <v>4</v>
+      </c>
+      <c r="R486" s="7"/>
+    </row>
+    <row r="487" spans="1:18">
+      <c r="A487" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="B487" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C487" s="2">
+        <v>720</v>
+      </c>
+      <c r="D487" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E487" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_072N@</v>
+      </c>
+      <c r="F487" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_072D@</v>
+      </c>
+      <c r="G487" s="5">
+        <v>720</v>
+      </c>
+      <c r="H487" s="8">
+        <v>0</v>
+      </c>
+      <c r="I487" s="8">
+        <v>50</v>
+      </c>
+      <c r="J487" s="7">
+        <v>70</v>
+      </c>
+      <c r="K487" s="7">
+        <v>30</v>
+      </c>
+      <c r="L487" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_072</v>
+      </c>
+      <c r="N487" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_072</v>
+      </c>
+      <c r="O487" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P487" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q487" s="2">
+        <v>4</v>
+      </c>
+      <c r="R487" s="7"/>
+    </row>
+    <row r="488" spans="1:18">
+      <c r="A488" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="B488" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C488" s="7">
+        <v>730</v>
+      </c>
+      <c r="D488" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E488" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_073N@</v>
+      </c>
+      <c r="F488" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_073D@</v>
+      </c>
+      <c r="G488" s="8">
+        <v>730</v>
+      </c>
+      <c r="H488" s="8">
+        <v>0</v>
+      </c>
+      <c r="I488" s="8">
+        <v>50</v>
+      </c>
+      <c r="J488" s="7">
+        <v>70</v>
+      </c>
+      <c r="K488" s="7">
+        <v>30</v>
+      </c>
+      <c r="L488" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_073</v>
+      </c>
+      <c r="N488" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_073</v>
+      </c>
+      <c r="O488" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P488" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q488" s="2">
+        <v>4</v>
+      </c>
+      <c r="R488" s="7"/>
+    </row>
+    <row r="489" spans="1:18">
+      <c r="A489" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="B489" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C489" s="2">
+        <v>740</v>
+      </c>
+      <c r="D489" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E489" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_074N@</v>
+      </c>
+      <c r="F489" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_074D@</v>
+      </c>
+      <c r="G489" s="5">
+        <v>740</v>
+      </c>
+      <c r="H489" s="8">
+        <v>0</v>
+      </c>
+      <c r="I489" s="8">
+        <v>50</v>
+      </c>
+      <c r="J489" s="7">
+        <v>70</v>
+      </c>
+      <c r="K489" s="7">
+        <v>30</v>
+      </c>
+      <c r="L489" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_074</v>
+      </c>
+      <c r="N489" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_074</v>
+      </c>
+      <c r="O489" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P489" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q489" s="2">
+        <v>4</v>
+      </c>
+      <c r="R489" s="7"/>
+    </row>
+    <row r="490" spans="1:18">
+      <c r="A490" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="B490" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C490" s="7">
+        <v>750</v>
+      </c>
+      <c r="D490" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E490" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_075N@</v>
+      </c>
+      <c r="F490" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_075D@</v>
+      </c>
+      <c r="G490" s="8">
+        <v>750</v>
+      </c>
+      <c r="H490" s="8">
+        <v>0</v>
+      </c>
+      <c r="I490" s="8">
+        <v>50</v>
+      </c>
+      <c r="J490" s="7">
+        <v>70</v>
+      </c>
+      <c r="K490" s="7">
+        <v>30</v>
+      </c>
+      <c r="L490" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_075</v>
+      </c>
+      <c r="N490" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_075</v>
+      </c>
+      <c r="O490" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P490" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q490" s="2">
+        <v>4</v>
+      </c>
+      <c r="R490" s="7"/>
+    </row>
+    <row r="491" spans="1:18">
+      <c r="A491" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="B491" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C491" s="2">
+        <v>760</v>
+      </c>
+      <c r="D491" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E491" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_076N@</v>
+      </c>
+      <c r="F491" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_076D@</v>
+      </c>
+      <c r="G491" s="5">
+        <v>760</v>
+      </c>
+      <c r="H491" s="8">
+        <v>0</v>
+      </c>
+      <c r="I491" s="8">
+        <v>50</v>
+      </c>
+      <c r="J491" s="7">
+        <v>70</v>
+      </c>
+      <c r="K491" s="7">
+        <v>30</v>
+      </c>
+      <c r="L491" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_076</v>
+      </c>
+      <c r="N491" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_076</v>
+      </c>
+      <c r="O491" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P491" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q491" s="2">
+        <v>3</v>
+      </c>
+      <c r="R491" s="7"/>
+    </row>
+    <row r="492" spans="1:18">
+      <c r="A492" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="B492" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C492" s="7">
+        <v>770</v>
+      </c>
+      <c r="D492" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E492" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_077N@</v>
+      </c>
+      <c r="F492" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_077D@</v>
+      </c>
+      <c r="G492" s="8">
+        <v>770</v>
+      </c>
+      <c r="H492" s="8">
+        <v>0</v>
+      </c>
+      <c r="I492" s="8">
+        <v>50</v>
+      </c>
+      <c r="J492" s="7">
+        <v>70</v>
+      </c>
+      <c r="K492" s="7">
+        <v>30</v>
+      </c>
+      <c r="L492" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_077</v>
+      </c>
+      <c r="N492" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_077</v>
+      </c>
+      <c r="O492" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P492" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q492" s="2">
+        <v>3</v>
+      </c>
+      <c r="R492" s="7"/>
+    </row>
+    <row r="493" spans="1:18">
+      <c r="A493" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="B493" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C493" s="2">
+        <v>780</v>
+      </c>
+      <c r="D493" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E493" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_078N@</v>
+      </c>
+      <c r="F493" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_078D@</v>
+      </c>
+      <c r="G493" s="5">
+        <v>780</v>
+      </c>
+      <c r="H493" s="8">
+        <v>0</v>
+      </c>
+      <c r="I493" s="8">
+        <v>50</v>
+      </c>
+      <c r="J493" s="7">
+        <v>70</v>
+      </c>
+      <c r="K493" s="7">
+        <v>30</v>
+      </c>
+      <c r="L493" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_078</v>
+      </c>
+      <c r="N493" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_078</v>
+      </c>
+      <c r="O493" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P493" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q493" s="2">
+        <v>3</v>
+      </c>
+      <c r="R493" s="7"/>
+    </row>
+    <row r="494" spans="1:18">
+      <c r="A494" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="B494" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C494" s="7">
+        <v>790</v>
+      </c>
+      <c r="D494" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E494" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_079N@</v>
+      </c>
+      <c r="F494" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_079D@</v>
+      </c>
+      <c r="G494" s="8">
+        <v>790</v>
+      </c>
+      <c r="H494" s="8">
+        <v>0</v>
+      </c>
+      <c r="I494" s="8">
+        <v>50</v>
+      </c>
+      <c r="J494" s="7">
+        <v>70</v>
+      </c>
+      <c r="K494" s="7">
+        <v>30</v>
+      </c>
+      <c r="L494" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_079</v>
+      </c>
+      <c r="N494" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_079</v>
+      </c>
+      <c r="O494" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P494" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q494" s="2">
+        <v>4</v>
+      </c>
+      <c r="R494" s="7"/>
+    </row>
+    <row r="495" spans="1:18">
+      <c r="A495" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B495" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C495" s="2">
+        <v>800</v>
+      </c>
+      <c r="D495" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E495" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_080N@</v>
+      </c>
+      <c r="F495" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_080D@</v>
+      </c>
+      <c r="G495" s="5">
+        <v>800</v>
+      </c>
+      <c r="H495" s="8">
+        <v>0</v>
+      </c>
+      <c r="I495" s="8">
+        <v>50</v>
+      </c>
+      <c r="J495" s="7">
+        <v>70</v>
+      </c>
+      <c r="K495" s="7">
+        <v>30</v>
+      </c>
+      <c r="L495" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_080</v>
+      </c>
+      <c r="N495" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_080</v>
+      </c>
+      <c r="O495" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P495" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q495" s="2">
+        <v>4</v>
+      </c>
+      <c r="R495" s="7"/>
+    </row>
+    <row r="496" spans="1:18">
+      <c r="A496" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="B496" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C496" s="7">
+        <v>810</v>
+      </c>
+      <c r="D496" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E496" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_081N@</v>
+      </c>
+      <c r="F496" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_081D@</v>
+      </c>
+      <c r="G496" s="8">
+        <v>810</v>
+      </c>
+      <c r="H496" s="8">
+        <v>0</v>
+      </c>
+      <c r="I496" s="8">
+        <v>50</v>
+      </c>
+      <c r="J496" s="7">
+        <v>70</v>
+      </c>
+      <c r="K496" s="7">
+        <v>30</v>
+      </c>
+      <c r="L496" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_081</v>
+      </c>
+      <c r="N496" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_081</v>
+      </c>
+      <c r="O496" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P496" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q496" s="2">
+        <v>4</v>
+      </c>
+      <c r="R496" s="7"/>
+    </row>
+    <row r="497" spans="1:18">
+      <c r="A497" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="B497" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C497" s="2">
+        <v>820</v>
+      </c>
+      <c r="D497" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E497" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_082N@</v>
+      </c>
+      <c r="F497" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_082D@</v>
+      </c>
+      <c r="G497" s="5">
+        <v>820</v>
+      </c>
+      <c r="H497" s="8">
+        <v>0</v>
+      </c>
+      <c r="I497" s="8">
+        <v>50</v>
+      </c>
+      <c r="J497" s="7">
+        <v>70</v>
+      </c>
+      <c r="K497" s="7">
+        <v>30</v>
+      </c>
+      <c r="L497" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_082</v>
+      </c>
+      <c r="N497" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_082</v>
+      </c>
+      <c r="O497" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P497" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q497" s="2">
+        <v>4</v>
+      </c>
+      <c r="R497" s="7"/>
+    </row>
+    <row r="498" spans="1:18">
+      <c r="A498" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="B498" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C498" s="7">
+        <v>830</v>
+      </c>
+      <c r="D498" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E498" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_083N@</v>
+      </c>
+      <c r="F498" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_083D@</v>
+      </c>
+      <c r="G498" s="8">
+        <v>830</v>
+      </c>
+      <c r="H498" s="8">
+        <v>0</v>
+      </c>
+      <c r="I498" s="8">
+        <v>50</v>
+      </c>
+      <c r="J498" s="7">
+        <v>70</v>
+      </c>
+      <c r="K498" s="7">
+        <v>30</v>
+      </c>
+      <c r="L498" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_083</v>
+      </c>
+      <c r="N498" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_083</v>
+      </c>
+      <c r="O498" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P498" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q498" s="2">
+        <v>4</v>
+      </c>
+      <c r="R498" s="7"/>
+    </row>
+    <row r="499" spans="1:18">
+      <c r="A499" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="B499" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C499" s="2">
+        <v>840</v>
+      </c>
+      <c r="D499" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E499" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_084N@</v>
+      </c>
+      <c r="F499" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_084D@</v>
+      </c>
+      <c r="G499" s="5">
+        <v>840</v>
+      </c>
+      <c r="H499" s="8">
+        <v>0</v>
+      </c>
+      <c r="I499" s="8">
+        <v>50</v>
+      </c>
+      <c r="J499" s="7">
+        <v>70</v>
+      </c>
+      <c r="K499" s="7">
+        <v>30</v>
+      </c>
+      <c r="L499" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_084</v>
+      </c>
+      <c r="N499" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_084</v>
+      </c>
+      <c r="O499" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P499" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q499" s="2">
+        <v>4</v>
+      </c>
+      <c r="R499" s="7"/>
+    </row>
+    <row r="500" spans="1:18">
+      <c r="A500" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B500" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C500" s="7">
+        <v>850</v>
+      </c>
+      <c r="D500" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E500" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_085N@</v>
+      </c>
+      <c r="F500" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_085D@</v>
+      </c>
+      <c r="G500" s="8">
+        <v>850</v>
+      </c>
+      <c r="H500" s="8">
+        <v>0</v>
+      </c>
+      <c r="I500" s="8">
+        <v>50</v>
+      </c>
+      <c r="J500" s="7">
+        <v>70</v>
+      </c>
+      <c r="K500" s="7">
+        <v>30</v>
+      </c>
+      <c r="L500" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_085</v>
+      </c>
+      <c r="N500" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_085</v>
+      </c>
+      <c r="O500" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P500" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q500" s="2">
+        <v>4</v>
+      </c>
+      <c r="R500" s="7"/>
+    </row>
+    <row r="501" spans="1:18">
+      <c r="A501" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B501" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C501" s="2">
+        <v>860</v>
+      </c>
+      <c r="D501" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E501" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_086N@</v>
+      </c>
+      <c r="F501" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_086D@</v>
+      </c>
+      <c r="G501" s="5">
+        <v>860</v>
+      </c>
+      <c r="H501" s="8">
+        <v>0</v>
+      </c>
+      <c r="I501" s="8">
+        <v>50</v>
+      </c>
+      <c r="J501" s="7">
+        <v>70</v>
+      </c>
+      <c r="K501" s="7">
+        <v>30</v>
+      </c>
+      <c r="L501" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_086</v>
+      </c>
+      <c r="N501" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_086</v>
+      </c>
+      <c r="O501" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P501" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q501" s="2">
+        <v>4</v>
+      </c>
+      <c r="R501" s="7"/>
+    </row>
+    <row r="502" spans="1:18">
+      <c r="A502" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="B502" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C502" s="7">
+        <v>870</v>
+      </c>
+      <c r="D502" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E502" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_087N@</v>
+      </c>
+      <c r="F502" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_087D@</v>
+      </c>
+      <c r="G502" s="8">
+        <v>870</v>
+      </c>
+      <c r="H502" s="8">
+        <v>0</v>
+      </c>
+      <c r="I502" s="8">
+        <v>50</v>
+      </c>
+      <c r="J502" s="7">
+        <v>70</v>
+      </c>
+      <c r="K502" s="7">
+        <v>30</v>
+      </c>
+      <c r="L502" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_087</v>
+      </c>
+      <c r="N502" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_087</v>
+      </c>
+      <c r="O502" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P502" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q502" s="2">
+        <v>4</v>
+      </c>
+      <c r="R502" s="7"/>
+    </row>
+    <row r="503" spans="1:18">
+      <c r="A503" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="B503" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C503" s="2">
+        <v>880</v>
+      </c>
+      <c r="D503" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E503" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_088N@</v>
+      </c>
+      <c r="F503" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_088D@</v>
+      </c>
+      <c r="G503" s="5">
+        <v>880</v>
+      </c>
+      <c r="H503" s="8">
+        <v>0</v>
+      </c>
+      <c r="I503" s="8">
+        <v>50</v>
+      </c>
+      <c r="J503" s="7">
+        <v>70</v>
+      </c>
+      <c r="K503" s="7">
+        <v>30</v>
+      </c>
+      <c r="L503" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_088</v>
+      </c>
+      <c r="N503" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_088</v>
+      </c>
+      <c r="O503" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P503" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q503" s="2">
+        <v>3</v>
+      </c>
+      <c r="R503" s="7"/>
+    </row>
+    <row r="504" spans="1:18">
+      <c r="A504" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="B504" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C504" s="7">
+        <v>890</v>
+      </c>
+      <c r="D504" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E504" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_089N@</v>
+      </c>
+      <c r="F504" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_089D@</v>
+      </c>
+      <c r="G504" s="8">
+        <v>890</v>
+      </c>
+      <c r="H504" s="8">
+        <v>0</v>
+      </c>
+      <c r="I504" s="8">
+        <v>50</v>
+      </c>
+      <c r="J504" s="7">
+        <v>70</v>
+      </c>
+      <c r="K504" s="7">
+        <v>30</v>
+      </c>
+      <c r="L504" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_089</v>
+      </c>
+      <c r="N504" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_089</v>
+      </c>
+      <c r="O504" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P504" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q504" s="2">
+        <v>3</v>
+      </c>
+      <c r="R504" s="7"/>
+    </row>
+    <row r="505" spans="1:18">
+      <c r="A505" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="B505" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C505" s="2">
+        <v>900</v>
+      </c>
+      <c r="D505" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="E505" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"N@")</f>
+        <v>@SR00_090N@</v>
+      </c>
+      <c r="F505" s="7" t="str">
+        <f>CONCATENATE("@S",표28[[#This Row],[id]],"D@")</f>
+        <v>@SR00_090D@</v>
+      </c>
+      <c r="G505" s="5">
+        <v>900</v>
+      </c>
+      <c r="H505" s="8">
+        <v>0</v>
+      </c>
+      <c r="I505" s="8">
+        <v>50</v>
+      </c>
+      <c r="J505" s="7">
+        <v>70</v>
+      </c>
+      <c r="K505" s="7">
+        <v>30</v>
+      </c>
+      <c r="L505" s="7" t="str">
+        <f>CONCATENATE("B",표28[[#This Row],[id]])</f>
+        <v>BR00_090</v>
+      </c>
+      <c r="N505" s="7" t="str">
+        <f>표28[[#This Row],[groupid]]</f>
+        <v>BR00_090</v>
+      </c>
+      <c r="O505" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P505" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q505" s="2">
+        <v>3</v>
+      </c>
+      <c r="R505" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -27590,7 +30236,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -27628,8 +30274,8 @@
       <c r="C2">
         <v>5200</v>
       </c>
-      <c r="D2">
-        <v>3.3361999999999998</v>
+      <c r="D2" s="9">
+        <v>6.4396000000000004</v>
       </c>
       <c r="E2">
         <v>86</v>
@@ -27645,8 +30291,8 @@
       <c r="C3">
         <v>5300</v>
       </c>
-      <c r="D3">
-        <v>36.895000000000003</v>
+      <c r="D3" s="10">
+        <v>53.220199999999998</v>
       </c>
       <c r="E3">
         <v>2001</v>
@@ -27662,8 +30308,8 @@
       <c r="C4">
         <v>5500</v>
       </c>
-      <c r="D4" s="4">
-        <v>1017.7</v>
+      <c r="D4" s="11">
+        <v>1301.57</v>
       </c>
       <c r="E4">
         <v>108544.00000000048</v>
@@ -27679,8 +30325,8 @@
       <c r="C5">
         <v>5700</v>
       </c>
-      <c r="D5">
-        <v>39766</v>
+      <c r="D5" s="12">
+        <v>47625</v>
       </c>
       <c r="E5">
         <v>7733248</v>
@@ -27696,8 +30342,8 @@
       <c r="C6">
         <v>6100</v>
       </c>
-      <c r="D6">
-        <v>15589731</v>
+      <c r="D6" s="13">
+        <v>17892498</v>
       </c>
       <c r="E6">
         <v>6056866302</v>
@@ -27713,8 +30359,8 @@
       <c r="C7">
         <v>6300</v>
       </c>
-      <c r="D7">
-        <v>4990733267</v>
+      <c r="D7" s="14">
+        <v>5564051276</v>
       </c>
       <c r="E7">
         <v>3509157065962</v>
@@ -27730,8 +30376,8 @@
       <c r="C8">
         <v>6700</v>
       </c>
-      <c r="D8">
-        <v>1677322427419</v>
+      <c r="D8" s="15">
+        <v>1831700929713</v>
       </c>
       <c r="E8">
         <v>2005605675653396</v>
@@ -27747,8 +30393,8 @@
       <c r="C9">
         <v>6900</v>
       </c>
-      <c r="D9">
-        <v>1312779264637361.5</v>
+      <c r="D9" s="16">
+        <v>1411744908409495.7</v>
       </c>
       <c r="E9">
         <v>2.6376361699820129E+18</v>
@@ -27764,7 +30410,7 @@
       <c r="C10">
         <v>7300</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="17">
         <v>1.9356116650602877E+18</v>
       </c>
       <c r="E10">

</xml_diff>